<commit_message>
Day 1 and Day 2
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bablove/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A296DB3B-D750-F440-AE8C-C019300B98C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77016ED0-43AC-485F-B146-6460AC874870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="940" windowWidth="27640" windowHeight="16200" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1426,6 +1426,9 @@
   </si>
   <si>
     <t xml:space="preserve">Youtube Channel: https://www.youtube.com/channel/UCQHLxxBFrbfdrk1jF0moTpw </t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -1857,18 +1860,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26">
+    <row r="1" spans="1:3" ht="24.6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1890,9 +1893,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="C5" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" ht="21">
       <c r="A6" s="5" t="s">
@@ -1902,7 +1903,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="21">
@@ -1913,7 +1914,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="21">
@@ -1924,7 +1925,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21">
@@ -1935,7 +1936,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="21">
@@ -1946,7 +1947,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="21">
@@ -1957,7 +1958,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="21">
@@ -1968,7 +1969,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="21">
@@ -1979,7 +1980,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21">
@@ -2034,7 +2035,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="21">
@@ -2292,16 +2293,12 @@
     </row>
     <row r="42" spans="1:3" ht="21">
       <c r="B42" s="7"/>
-      <c r="C42" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="C42" s="4"/>
     </row>
     <row r="43" spans="1:3" ht="21">
       <c r="A43" s="5"/>
       <c r="B43" s="7"/>
-      <c r="C43" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="C43" s="4"/>
     </row>
     <row r="44" spans="1:3" ht="21">
       <c r="A44" s="8" t="s">

</xml_diff>

<commit_message>
Day 3 and Day 4
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77016ED0-43AC-485F-B146-6460AC874870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AD4851-6375-4508-8513-F34B54812691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1498,12 +1498,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1519,7 +1537,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1543,6 +1561,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1860,7 +1887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -1902,7 +1929,7 @@
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="11" t="s">
         <v>465</v>
       </c>
     </row>
@@ -1913,7 +1940,7 @@
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="11" t="s">
         <v>465</v>
       </c>
     </row>
@@ -1924,7 +1951,7 @@
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="11" t="s">
         <v>465</v>
       </c>
     </row>
@@ -1935,7 +1962,7 @@
       <c r="B9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="11" t="s">
         <v>465</v>
       </c>
     </row>
@@ -1946,7 +1973,7 @@
       <c r="B10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="11" t="s">
         <v>465</v>
       </c>
     </row>
@@ -1957,7 +1984,7 @@
       <c r="B11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="11" t="s">
         <v>465</v>
       </c>
     </row>
@@ -1968,7 +1995,7 @@
       <c r="B12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="11" t="s">
         <v>465</v>
       </c>
     </row>
@@ -1979,7 +2006,7 @@
       <c r="B13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="12" t="s">
         <v>465</v>
       </c>
     </row>
@@ -1990,8 +2017,8 @@
       <c r="B14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>4</v>
+      <c r="C14" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="21">
@@ -2001,8 +2028,8 @@
       <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>4</v>
+      <c r="C15" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="21">
@@ -2012,8 +2039,8 @@
       <c r="B16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>4</v>
+      <c r="C16" s="13" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="21">
@@ -2023,8 +2050,8 @@
       <c r="B17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>4</v>
+      <c r="C17" s="13" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="21">
@@ -2034,7 +2061,7 @@
       <c r="B18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="12" t="s">
         <v>465</v>
       </c>
     </row>
@@ -2045,8 +2072,8 @@
       <c r="B19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>4</v>
+      <c r="C19" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="21">
@@ -7375,5 +7402,6 @@
     <hyperlink ref="B2" r:id="rId446" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId447"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day 11 and Day 12
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8017E40F-7375-42B7-9431-EBED0F551AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68972E4E-8CD2-44E0-B051-8D715F122F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1905,8 +1905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="B29" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2310,8 +2310,8 @@
       <c r="B39" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>4</v>
+      <c r="C39" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="21">
@@ -2321,8 +2321,8 @@
       <c r="B40" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>4</v>
+      <c r="C40" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="21">
@@ -2332,8 +2332,8 @@
       <c r="B41" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>4</v>
+      <c r="C41" s="13" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 13 and Day 14
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68972E4E-8CD2-44E0-B051-8D715F122F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B0A337-CE7C-4AF5-9C30-4090C3D21F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1905,8 +1905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B29" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="B36" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2352,8 +2352,8 @@
       <c r="B44" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>4</v>
+      <c r="C44" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="21">
@@ -2363,8 +2363,8 @@
       <c r="B45" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>4</v>
+      <c r="C45" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="21">
@@ -2374,8 +2374,8 @@
       <c r="B46" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>4</v>
+      <c r="C46" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="21">
@@ -2385,8 +2385,8 @@
       <c r="B47" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>4</v>
+      <c r="C47" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 15 and Day 16
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B0A337-CE7C-4AF5-9C30-4090C3D21F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F97C7E4-4BEF-4074-83D9-298809564254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1498,7 +1498,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1535,6 +1535,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1549,7 +1555,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1586,6 +1592,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1905,8 +1914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B36" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="B42" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2396,8 +2405,8 @@
       <c r="B48" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>4</v>
+      <c r="C48" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="21">
@@ -2407,8 +2416,8 @@
       <c r="B49" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>4</v>
+      <c r="C49" s="16" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="21">
@@ -2418,8 +2427,8 @@
       <c r="B50" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C50" s="4" t="s">
-        <v>4</v>
+      <c r="C50" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="21">
@@ -2429,8 +2438,8 @@
       <c r="B51" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>4</v>
+      <c r="C51" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 17 and Day 18
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F97C7E4-4BEF-4074-83D9-298809564254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B28FA5-F584-4985-A6E4-79AE3420C80E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1914,7 +1914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B42" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B45" workbookViewId="0">
       <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
@@ -2449,8 +2449,8 @@
       <c r="B52" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>4</v>
+      <c r="C52" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="21">
@@ -2460,8 +2460,8 @@
       <c r="B53" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>4</v>
+      <c r="C53" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 21 and Day 22
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E69207-5691-40F5-B26C-AC2C07E29AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3AE770-008B-45C6-9CCC-0DB9060BE97D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1915,7 +1915,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2553,8 +2553,8 @@
       <c r="B63" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C63" s="4" t="s">
-        <v>4</v>
+      <c r="C63" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="21">
@@ -2564,8 +2564,8 @@
       <c r="B64" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C64" s="4" t="s">
-        <v>4</v>
+      <c r="C64" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="21">
@@ -2575,8 +2575,8 @@
       <c r="B65" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>4</v>
+      <c r="C65" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="21">
@@ -2586,8 +2586,8 @@
       <c r="B66" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C66" s="4" t="s">
-        <v>4</v>
+      <c r="C66" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="21">
@@ -2597,8 +2597,8 @@
       <c r="B67" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C67" s="4" t="s">
-        <v>4</v>
+      <c r="C67" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 23, 24 and 25
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3AE770-008B-45C6-9CCC-0DB9060BE97D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6536A561-AF81-4634-95BB-E85F9C1BF1AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1498,7 +1498,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1541,6 +1541,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1555,7 +1561,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1595,6 +1601,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1904,7 +1913,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1914,8 +1923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2608,8 +2617,8 @@
       <c r="B68" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>4</v>
+      <c r="C68" s="17" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="21">
@@ -2619,8 +2628,8 @@
       <c r="B69" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C69" s="4" t="s">
-        <v>4</v>
+      <c r="C69" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="21">
@@ -2630,8 +2639,8 @@
       <c r="B70" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C70" s="4" t="s">
-        <v>4</v>
+      <c r="C70" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="21">
@@ -2641,7 +2650,7 @@
       <c r="B71" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C71" s="15" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2652,8 +2661,8 @@
       <c r="B72" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C72" s="4" t="s">
-        <v>4</v>
+      <c r="C72" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 27 and 28
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD9ACE1-2337-454E-80F1-2E9DE955534C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53C8AC8-8E69-4F8E-A3FA-E44EB63A1254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1923,8 +1923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2694,8 +2694,8 @@
       <c r="B75" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C75" s="4" t="s">
-        <v>4</v>
+      <c r="C75" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="21">
@@ -2705,8 +2705,8 @@
       <c r="B76" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C76" s="4" t="s">
-        <v>4</v>
+      <c r="C76" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="21">
@@ -2716,8 +2716,8 @@
       <c r="B77" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C77" s="4" t="s">
-        <v>4</v>
+      <c r="C77" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 29 and Day 30
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53C8AC8-8E69-4F8E-A3FA-E44EB63A1254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66361DCE-8356-474B-A5E0-81C6721B072D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1923,8 +1923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2727,8 +2727,8 @@
       <c r="B78" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C78" s="4" t="s">
-        <v>4</v>
+      <c r="C78" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="21">
@@ -2738,8 +2738,8 @@
       <c r="B79" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C79" s="4" t="s">
-        <v>4</v>
+      <c r="C79" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="21">
@@ -2749,8 +2749,8 @@
       <c r="B80" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C80" s="4" t="s">
-        <v>4</v>
+      <c r="C80" s="16" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="21">
@@ -2760,8 +2760,8 @@
       <c r="B81" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C81" s="4" t="s">
-        <v>4</v>
+      <c r="C81" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="21">
@@ -2771,8 +2771,8 @@
       <c r="B82" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C82" s="4" t="s">
-        <v>4</v>
+      <c r="C82" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 31 and 32
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66361DCE-8356-474B-A5E0-81C6721B072D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EC6D41-DCF9-4882-8B02-0731E9CC96CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1924,7 +1924,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2782,8 +2782,8 @@
       <c r="B83" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C83" s="4" t="s">
-        <v>4</v>
+      <c r="C83" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="21">
@@ -2793,8 +2793,8 @@
       <c r="B84" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C84" s="4" t="s">
-        <v>4</v>
+      <c r="C84" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="21">
@@ -2804,8 +2804,8 @@
       <c r="B85" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C85" s="4" t="s">
-        <v>4</v>
+      <c r="C85" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="21">
@@ -2815,8 +2815,8 @@
       <c r="B86" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C86" s="4" t="s">
-        <v>4</v>
+      <c r="C86" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 34, 35 and 36
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EC6D41-DCF9-4882-8B02-0731E9CC96CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCF6302-C8C2-43FE-8BC9-4AFD64FC528A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1923,8 +1923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2826,8 +2826,8 @@
       <c r="B87" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C87" s="4" t="s">
-        <v>4</v>
+      <c r="C87" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="21">
@@ -2837,8 +2837,8 @@
       <c r="B88" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C88" s="4" t="s">
-        <v>4</v>
+      <c r="C88" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="21">
@@ -2848,8 +2848,8 @@
       <c r="B89" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C89" s="4" t="s">
-        <v>4</v>
+      <c r="C89" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="21">
@@ -2859,8 +2859,8 @@
       <c r="B90" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C90" s="4" t="s">
-        <v>4</v>
+      <c r="C90" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="21">
@@ -7066,376 +7066,376 @@
     <hyperlink ref="B84" r:id="rId74" xr:uid="{789FFFAC-8B7E-0540-98B8-856430EB56F8}"/>
     <hyperlink ref="B85" r:id="rId75" xr:uid="{4A0E959E-22F4-6948-A819-76FE76AB9F6D}"/>
     <hyperlink ref="B86" r:id="rId76" xr:uid="{78B76678-D8EE-9745-98B1-DF7A76EA3B10}"/>
-    <hyperlink ref="B87" r:id="rId77" xr:uid="{62982242-1D19-1544-8653-8E25E9BF4505}"/>
-    <hyperlink ref="B88" r:id="rId78" xr:uid="{8E3D4BDF-9F8F-0542-BFD8-C3CE3BF396E6}"/>
-    <hyperlink ref="B89" r:id="rId79" xr:uid="{A3D51762-65A1-9A44-B619-D1D98A7F403B}"/>
-    <hyperlink ref="B90" r:id="rId80" xr:uid="{ED0F5FC7-0066-EB44-8FCF-460600DADB02}"/>
-    <hyperlink ref="B91" r:id="rId81" xr:uid="{2D956AC4-4774-7446-8473-C4CE00E33C17}"/>
-    <hyperlink ref="B92" r:id="rId82" xr:uid="{C8C607BB-1FEE-FA47-9E3E-6C0BCE978B7F}"/>
-    <hyperlink ref="B93" r:id="rId83" xr:uid="{B9AC5194-6D36-684A-A5C4-BEE11037599F}"/>
-    <hyperlink ref="B94" r:id="rId84" xr:uid="{AB28D9E6-890C-F14A-A5FB-2303BE319968}"/>
-    <hyperlink ref="B95" r:id="rId85" xr:uid="{1F507CBC-4056-AD46-9314-95ECBB9D799D}"/>
-    <hyperlink ref="B96" r:id="rId86" xr:uid="{F152A9AF-5CBA-EC44-A9CF-07AB481435AB}"/>
-    <hyperlink ref="B97" r:id="rId87" xr:uid="{346CA74F-60B7-0A4B-A612-9184D4DCFF62}"/>
-    <hyperlink ref="B98" r:id="rId88" xr:uid="{8C653CB1-4954-754F-8D46-F09141A2FCDB}"/>
-    <hyperlink ref="B101" r:id="rId89" xr:uid="{5989F693-2A61-A346-8395-8674307A4CC2}"/>
-    <hyperlink ref="B102" r:id="rId90" xr:uid="{3AD10C9E-4F6D-DE48-92F3-531A586520C6}"/>
-    <hyperlink ref="B103" r:id="rId91" xr:uid="{4FA217C0-A1F3-904E-8FEA-EA4941273A67}"/>
-    <hyperlink ref="B104" r:id="rId92" xr:uid="{A297BBC0-FA0D-2D46-9C49-3932193EF1D3}"/>
-    <hyperlink ref="B106" r:id="rId93" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance." xr:uid="{DCD751DE-E440-F346-B6FD-CBD072217214}"/>
-    <hyperlink ref="B107" r:id="rId94" xr:uid="{B2FD38B9-1E2B-8140-8291-F45734C98145}"/>
-    <hyperlink ref="B108" r:id="rId95" xr:uid="{C76888B3-18AC-9B48-9E2A-64A7DF0902B7}"/>
-    <hyperlink ref="B109" r:id="rId96" xr:uid="{18A79860-6C9E-A941-8D6C-360B9913E941}"/>
-    <hyperlink ref="B110" r:id="rId97" xr:uid="{C0DDFD68-CBC1-0F4A-AF40-ACF36BBC8453}"/>
-    <hyperlink ref="B111" r:id="rId98" xr:uid="{3E0BF737-E42E-C946-B32C-06882E0BA6FF}"/>
-    <hyperlink ref="B113" r:id="rId99" xr:uid="{862F9782-C57B-2848-A2D9-EB7B52FB7EC7}"/>
-    <hyperlink ref="B114" r:id="rId100" xr:uid="{230D7A6A-D2C5-C140-9A65-B1F407D22062}"/>
-    <hyperlink ref="B115" r:id="rId101" xr:uid="{BDC2BA28-4562-984E-8282-1126BF952EAF}"/>
-    <hyperlink ref="B116" r:id="rId102" xr:uid="{B53A5F28-6DED-3D47-8679-F78D3DDEFF01}"/>
-    <hyperlink ref="B117" r:id="rId103" xr:uid="{C57D0CC7-DA2F-0948-9BCE-F19C20C7D981}"/>
-    <hyperlink ref="B118" r:id="rId104" xr:uid="{117878E5-B8C8-254B-8ED6-014B4B7A8126}"/>
-    <hyperlink ref="B119" r:id="rId105" xr:uid="{B7CC0756-74F2-D54D-BDEE-9DA394DD7168}"/>
-    <hyperlink ref="B120" r:id="rId106" xr:uid="{837EF472-CCC2-CF47-A8A8-238E56F722CE}"/>
-    <hyperlink ref="B121" r:id="rId107" xr:uid="{3608F267-6AA0-624B-B243-7DDD317E9F08}"/>
-    <hyperlink ref="B122" r:id="rId108" xr:uid="{0B6123E6-0472-374B-ACA7-6914CD7918E8}"/>
-    <hyperlink ref="B123" r:id="rId109" xr:uid="{D3971CEB-C53E-B04B-9C32-1803182B5DC5}"/>
-    <hyperlink ref="B124" r:id="rId110" xr:uid="{7CF5013A-643E-1643-93A1-A2F1500D2A23}"/>
-    <hyperlink ref="B125" r:id="rId111" xr:uid="{2A6BE7E5-D818-6843-8C3E-99EA2BFE0FB2}"/>
-    <hyperlink ref="B126" r:id="rId112" xr:uid="{E718F544-96DF-A04E-8DFB-7639DA3EA57C}"/>
-    <hyperlink ref="B127" r:id="rId113" xr:uid="{B0C2F065-424A-7345-A864-346ECD98D749}"/>
-    <hyperlink ref="B128" r:id="rId114" xr:uid="{B4E26955-5C3F-804E-B19A-11260310AFB3}"/>
-    <hyperlink ref="B129" r:id="rId115" xr:uid="{6F299BB5-8E82-0240-A9A3-6829CE3ABCBF}"/>
-    <hyperlink ref="B130" r:id="rId116" xr:uid="{A42CA32F-2196-1840-A53D-E5073237C68D}"/>
-    <hyperlink ref="B131" r:id="rId117" xr:uid="{7ECF6EF4-962E-4642-9B1C-C3B70674793E}"/>
-    <hyperlink ref="B132" r:id="rId118" xr:uid="{2A109178-6B60-164E-9D25-42B3282137E3}"/>
-    <hyperlink ref="B133" r:id="rId119" xr:uid="{B3D38BD0-A6A1-8D41-8405-45E1BEEEEF06}"/>
-    <hyperlink ref="B134" r:id="rId120" xr:uid="{A1C26612-D040-2A41-A6A6-A8F2490C0A43}"/>
-    <hyperlink ref="B135" r:id="rId121" xr:uid="{C476E807-64CB-F44A-A23D-D21EBF6D001D}"/>
-    <hyperlink ref="B136" r:id="rId122" xr:uid="{9A414D55-D4A1-F147-9207-61B597D57136}"/>
-    <hyperlink ref="B105" r:id="rId123" xr:uid="{18B028A7-9B6F-D841-8548-924D70530779}"/>
-    <hyperlink ref="B112" r:id="rId124" xr:uid="{6D3E75EF-733F-7A4B-81C8-AEF6CB6335F0}"/>
-    <hyperlink ref="B139" r:id="rId125" xr:uid="{C9EB2682-BE0B-934B-B0B4-1DD1A1502647}"/>
-    <hyperlink ref="B140" r:id="rId126" xr:uid="{2992FED9-2B78-A342-92AA-E7C0F882FF17}"/>
-    <hyperlink ref="B141" r:id="rId127" xr:uid="{0084DA6F-EC84-BD48-BDA8-EBACA3BB3B3E}"/>
-    <hyperlink ref="B142" r:id="rId128" xr:uid="{30F2D415-4B2C-384C-8EAE-2CC71CB518E2}"/>
-    <hyperlink ref="B143" r:id="rId129" xr:uid="{40734C88-7C5B-9747-86D1-03463D9AD41A}"/>
-    <hyperlink ref="B144" r:id="rId130" xr:uid="{1040D22F-6729-104A-A229-CBDCED93024A}"/>
-    <hyperlink ref="B145" r:id="rId131" xr:uid="{E131FE61-FABF-8E4B-8EF0-F68379D8F836}"/>
-    <hyperlink ref="B146" r:id="rId132" xr:uid="{B2129272-1351-3745-883B-E6A7115450C8}"/>
-    <hyperlink ref="B147" r:id="rId133" xr:uid="{C8B2DEF0-2B69-C84E-8013-0B6F03FFC250}"/>
-    <hyperlink ref="B148" r:id="rId134" xr:uid="{536AC5CF-712F-BF48-94A9-D0E7DC013020}"/>
-    <hyperlink ref="B149" r:id="rId135" xr:uid="{2DABC9C7-43D4-1249-AF9B-5FA4552611CB}"/>
-    <hyperlink ref="B150" r:id="rId136" xr:uid="{DA62E73A-B495-F94A-BECE-D42E4CBF074A}"/>
-    <hyperlink ref="B151" r:id="rId137" xr:uid="{7F5E6966-850D-4F49-B2A5-678365713F28}"/>
-    <hyperlink ref="B152" r:id="rId138" xr:uid="{E9C4286D-8493-9A47-8B8C-09583FA72B70}"/>
-    <hyperlink ref="B153" r:id="rId139" xr:uid="{9EB0123C-84AE-1C4D-BA1A-C28CFB8EFB89}"/>
-    <hyperlink ref="B154" r:id="rId140" xr:uid="{9D11FED4-328F-674E-889D-EC781DD1D791}"/>
-    <hyperlink ref="B155" r:id="rId141" xr:uid="{48AE72DB-397B-464D-88AD-B8058ED29CC1}"/>
-    <hyperlink ref="B156" r:id="rId142" xr:uid="{152D50E9-7448-F542-AC66-05D0AE66664C}"/>
-    <hyperlink ref="B157" r:id="rId143" xr:uid="{34E6AF1B-5FB1-3A4B-8938-1DCF80831DC2}"/>
-    <hyperlink ref="B158" r:id="rId144" xr:uid="{E7F8B7CA-49F4-1946-91EE-E7582BE4E5DA}"/>
-    <hyperlink ref="B159" r:id="rId145" xr:uid="{3590A994-B7A2-C14D-9BF8-7AC8FE9E7F0F}"/>
-    <hyperlink ref="B160" r:id="rId146" xr:uid="{0AAA4B0C-4921-C34D-B41E-D702FA860892}"/>
-    <hyperlink ref="B161" r:id="rId147" xr:uid="{5973FCA4-AE32-5248-A6ED-2694367332F1}"/>
-    <hyperlink ref="B162" r:id="rId148" xr:uid="{4C0F816E-F043-0C47-BF16-1CDAD88D2FF1}"/>
-    <hyperlink ref="B163" r:id="rId149" xr:uid="{A8E4C654-D0BD-8945-9F5C-B09F7BC114BE}"/>
-    <hyperlink ref="B166" r:id="rId150" xr:uid="{E3825C15-10BB-E24F-B229-983F651DA942}"/>
-    <hyperlink ref="B167" r:id="rId151" xr:uid="{46ECFC31-388C-6241-8FFE-DED6F2FC794A}"/>
-    <hyperlink ref="B168" r:id="rId152" xr:uid="{589E024D-3FE1-1048-890C-88289733F233}"/>
-    <hyperlink ref="B169" r:id="rId153" xr:uid="{CDA28F7A-7FC5-F74D-B27E-A6E0161D41D5}"/>
-    <hyperlink ref="B170" r:id="rId154" xr:uid="{DA6A0D92-DCEB-DA4F-8BBA-10FCD092838F}"/>
-    <hyperlink ref="B171" r:id="rId155" xr:uid="{955769DB-3256-254B-90DE-E1E01B272F8A}"/>
-    <hyperlink ref="B172" r:id="rId156" xr:uid="{DED7AC9B-40D7-0545-9D6F-6CD4F5FFE4C6}"/>
-    <hyperlink ref="B173" r:id="rId157" xr:uid="{6947A4E1-B6AA-6D4F-A6D8-8FA74FD02887}"/>
-    <hyperlink ref="B174" r:id="rId158" xr:uid="{EABF2012-5A90-0C4E-86F6-FDB5FA7770BE}"/>
-    <hyperlink ref="B177" r:id="rId159" xr:uid="{7F44CFE0-9ED1-A44D-B9EF-CF87BEB644FC}"/>
-    <hyperlink ref="B178" r:id="rId160" xr:uid="{CF6E0CF6-7A93-D84A-9CE0-5BDD51767416}"/>
-    <hyperlink ref="B179" r:id="rId161" xr:uid="{EFF8F154-60B8-B84B-84CA-32756BD6430F}"/>
-    <hyperlink ref="B180" r:id="rId162" xr:uid="{C8A3094E-E11B-2543-B05E-1D07048B2EBA}"/>
-    <hyperlink ref="B181" r:id="rId163" xr:uid="{9961E5F5-B5C6-0C4D-A1D0-D04D2A5D7DFD}"/>
-    <hyperlink ref="B182" r:id="rId164" xr:uid="{44E289EC-47DD-D94D-88C1-CB2F59C6C16A}"/>
-    <hyperlink ref="B183" r:id="rId165" xr:uid="{4161FC70-DD6D-684B-898A-A4711596B2D5}"/>
-    <hyperlink ref="B184" r:id="rId166" xr:uid="{B9CBE387-8E9A-ED48-8310-CF7D34FA690C}"/>
-    <hyperlink ref="B185" r:id="rId167" xr:uid="{5398097B-24FF-9543-8F02-33CE2860F1F7}"/>
-    <hyperlink ref="B186" r:id="rId168" xr:uid="{3B1FC30B-30C8-7B48-AF94-A81FB513F24F}"/>
-    <hyperlink ref="B187" r:id="rId169" xr:uid="{32B750D0-D7F2-694D-AB9B-25AFAFAFF17F}"/>
-    <hyperlink ref="B188" r:id="rId170" xr:uid="{400689DD-8E95-024E-976B-AACD8ED4E1A6}"/>
-    <hyperlink ref="B189" r:id="rId171" xr:uid="{28753DDE-E047-5D40-A30B-1103BE6DA08F}"/>
-    <hyperlink ref="B190" r:id="rId172" xr:uid="{6C5AA6CB-3D93-0740-AEED-9E6C218CF6CB}"/>
-    <hyperlink ref="B191" r:id="rId173" xr:uid="{03EAA2B9-D8B8-D642-BF24-380596D26B2E}"/>
-    <hyperlink ref="B192" r:id="rId174" xr:uid="{8C1719B4-37CC-484E-BDCE-A4272C07F91B}"/>
-    <hyperlink ref="B193" r:id="rId175" xr:uid="{6C198DA2-BB98-F940-8EF6-2FC8B7AE577A}"/>
-    <hyperlink ref="B194" r:id="rId176" xr:uid="{AB0EA311-A446-D046-A0EC-290B42068328}"/>
-    <hyperlink ref="B195" r:id="rId177" xr:uid="{DB913045-B9F6-6549-AA09-22B0CC5FDD21}"/>
-    <hyperlink ref="B196" r:id="rId178" xr:uid="{806469FD-617A-7445-AAB5-FB2FD2ED24EA}"/>
-    <hyperlink ref="B197" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{1A10544E-58CF-D04D-9FAF-2FEC6DB2B5D4}"/>
-    <hyperlink ref="B198" r:id="rId180" xr:uid="{5A0B6645-89FD-E044-A706-9FB890274C3C}"/>
-    <hyperlink ref="B199" r:id="rId181" xr:uid="{B42A3009-E8EB-EE44-885F-6699C17A0E0B}"/>
-    <hyperlink ref="B200" r:id="rId182" xr:uid="{ED3E48AB-E25B-3744-B024-E97B2A319B46}"/>
-    <hyperlink ref="B201" r:id="rId183" xr:uid="{C75D20A3-CBAE-2649-A3EE-E49177CFA343}"/>
-    <hyperlink ref="B202" r:id="rId184" xr:uid="{3863CA1B-D43E-1144-91A9-17C2DCF52A64}"/>
-    <hyperlink ref="B203" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{E9AF434E-4CAA-5D49-8AD3-889CDE2913D9}"/>
-    <hyperlink ref="B204" r:id="rId186" xr:uid="{1A0568E5-3A11-7F47-8001-82B05D7C2339}"/>
-    <hyperlink ref="B205" r:id="rId187" xr:uid="{F62B8AE4-9C4F-9544-8861-CD733C12F79E}"/>
-    <hyperlink ref="B206" r:id="rId188" xr:uid="{0F6A542C-44C9-5A4C-90BF-BC8C239877D2}"/>
-    <hyperlink ref="B207" r:id="rId189" xr:uid="{3ED28203-B1B5-4E46-AAF3-779EDD4AC03F}"/>
-    <hyperlink ref="B208" r:id="rId190" xr:uid="{4338B305-B52F-5540-9B51-B938FC6803A2}"/>
-    <hyperlink ref="B209" r:id="rId191" xr:uid="{DDEEED0F-A939-1E4F-B2FA-AD391A4A2874}"/>
-    <hyperlink ref="B210" r:id="rId192" xr:uid="{C2F20589-AD81-654C-94E5-E5B6C9FE27F6}"/>
-    <hyperlink ref="B211" r:id="rId193" xr:uid="{BBEB9DAC-E4AE-C04F-AA15-6356AFC57FDE}"/>
-    <hyperlink ref="B214" r:id="rId194" xr:uid="{6316566D-A10A-F849-9F25-B9ED4DA12BC7}"/>
-    <hyperlink ref="B215" r:id="rId195" xr:uid="{9D4DD895-FBA6-C849-A5BF-3B30755BD9C9}"/>
-    <hyperlink ref="B216" r:id="rId196" xr:uid="{475996DA-632A-BE49-AEA1-D4189FD614A1}"/>
-    <hyperlink ref="B217" r:id="rId197" xr:uid="{88E0C858-8468-884F-BB71-F6F176BD5FC2}"/>
-    <hyperlink ref="B218" r:id="rId198" xr:uid="{C1C5C8D0-7A06-3D4A-A85A-AAACC1B418C9}"/>
-    <hyperlink ref="B219" r:id="rId199" xr:uid="{D525D4B1-2857-1543-8CD9-196728321203}"/>
-    <hyperlink ref="B220" r:id="rId200" xr:uid="{51E3AB9B-04B2-C041-A2B3-37E3EB18013A}"/>
-    <hyperlink ref="B221" r:id="rId201" xr:uid="{7F7F0C9A-57B9-314F-959A-B8ACAFA5FD13}"/>
-    <hyperlink ref="B222" r:id="rId202" xr:uid="{3B029785-83B4-6140-8B70-CD892CFC87F6}"/>
-    <hyperlink ref="B223" r:id="rId203" xr:uid="{B0A390E6-D860-9F4E-B021-68949FE712F3}"/>
-    <hyperlink ref="B224" r:id="rId204" xr:uid="{49E9953D-52F6-BF47-8AAA-8E456F55576B}"/>
-    <hyperlink ref="B225" r:id="rId205" xr:uid="{9B812470-F419-A54E-8365-06A9B8864A30}"/>
-    <hyperlink ref="B226" r:id="rId206" xr:uid="{B6FB4107-1933-6D45-9EF4-4474E06CBE9D}"/>
-    <hyperlink ref="B227" r:id="rId207" xr:uid="{0F7C1D92-7BCB-D14D-A658-9599984E04E4}"/>
-    <hyperlink ref="B228" r:id="rId208" xr:uid="{6810428F-0A78-964C-A8C8-E1CD2E7C405D}"/>
-    <hyperlink ref="B229" r:id="rId209" xr:uid="{B40209F2-0D6E-364F-8AF6-F1D182509314}"/>
-    <hyperlink ref="B230" r:id="rId210" xr:uid="{96C53FA9-9FD3-2D4F-B292-3C9DEDFA806E}"/>
-    <hyperlink ref="B231" r:id="rId211" xr:uid="{918B420D-3678-FD46-9463-595E8ACC39E1}"/>
-    <hyperlink ref="B232" r:id="rId212" xr:uid="{851A7153-3B54-0E4A-A0A0-FCEB091AFE70}"/>
-    <hyperlink ref="B233" r:id="rId213" xr:uid="{C03AE9F8-09AE-C640-81A7-033BB06FB6AD}"/>
-    <hyperlink ref="B234" r:id="rId214" xr:uid="{35140DEB-52D2-4342-88D2-22BA061E5B48}"/>
-    <hyperlink ref="B235" r:id="rId215" xr:uid="{9714BC0B-3373-934C-B7A1-599F74F4FB9D}"/>
-    <hyperlink ref="B238" r:id="rId216" xr:uid="{5CB435B2-7FD2-1D44-9872-22B6A1EDC02B}"/>
-    <hyperlink ref="B239" r:id="rId217" xr:uid="{722D1D95-896B-4642-BABD-31DEDD237B49}"/>
-    <hyperlink ref="B240" r:id="rId218" xr:uid="{D686D1DC-13D6-284C-B606-E087FAF47399}"/>
-    <hyperlink ref="B241" r:id="rId219" xr:uid="{D22C2394-C3CB-8F4F-A010-2B13C8C84D1A}"/>
-    <hyperlink ref="B242" r:id="rId220" xr:uid="{3AE2F800-B66F-1A41-893B-978F6875FDC8}"/>
-    <hyperlink ref="B243" r:id="rId221" xr:uid="{2C939BDE-5298-5541-837B-8C59D53A33C1}"/>
-    <hyperlink ref="B244" r:id="rId222" xr:uid="{691C9BD8-69D3-DA4B-AEB6-AF827B4ACA9F}"/>
-    <hyperlink ref="B245" r:id="rId223" xr:uid="{B6891E82-7C4D-424D-9219-3C9FD08E0053}"/>
-    <hyperlink ref="B246" r:id="rId224" xr:uid="{67A1AE98-62D2-644D-AC13-6CD76CF53CC0}"/>
-    <hyperlink ref="B247" r:id="rId225" xr:uid="{B59D4881-2A82-8F4D-B151-1E796C4923C8}"/>
-    <hyperlink ref="B248" r:id="rId226" xr:uid="{B3CBD023-5EFD-6048-9B3F-89F0C65CBBF5}"/>
-    <hyperlink ref="B249" r:id="rId227" xr:uid="{53EC42C4-22F7-0445-A0AC-7275A59A2672}"/>
-    <hyperlink ref="B250" r:id="rId228" xr:uid="{A29575F3-CB24-5B4B-9538-D5212B2DC28B}"/>
-    <hyperlink ref="B251" r:id="rId229" xr:uid="{353A44DD-9E30-8F48-8E2B-8DAA07550470}"/>
-    <hyperlink ref="B252" r:id="rId230" xr:uid="{32AC291D-95A5-BE49-88E0-02677BF39CAC}"/>
-    <hyperlink ref="B253" r:id="rId231" xr:uid="{A84F22FF-AD10-A546-8998-B066C0EB2D5A}"/>
-    <hyperlink ref="B254" r:id="rId232" xr:uid="{4C5CAF84-9B94-FC44-8C6C-B3CC7257C1DB}"/>
-    <hyperlink ref="B255" r:id="rId233" xr:uid="{5DA775E2-C516-3B47-8C82-3CEE7CC0BDF9}"/>
-    <hyperlink ref="B256" r:id="rId234" xr:uid="{00B6AE5C-EF3F-0747-A280-3BF055362B4F}"/>
-    <hyperlink ref="B257" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{BCBD0A7E-F3D0-E840-9375-AFD37C5CD41A}"/>
-    <hyperlink ref="B258" r:id="rId236" xr:uid="{47ABDDDB-F95F-8049-9FB3-1E71A7376DDE}"/>
-    <hyperlink ref="B259" r:id="rId237" xr:uid="{70BADFC9-7399-234D-99F6-4C5F02397C26}"/>
-    <hyperlink ref="B260" r:id="rId238" xr:uid="{63348580-70EF-EC47-BF49-8ECE9560D54E}"/>
-    <hyperlink ref="B261" r:id="rId239" xr:uid="{D5BD96B3-9EAB-1B47-AC87-5C47F6AD7F40}"/>
-    <hyperlink ref="B262" r:id="rId240" xr:uid="{74791141-3FB8-7540-B45B-9541AF0AE371}"/>
-    <hyperlink ref="B263" r:id="rId241" xr:uid="{88D53CD6-262A-7247-8E58-FE9FFF7ECC40}"/>
-    <hyperlink ref="B264" r:id="rId242" xr:uid="{4338A14D-4F7D-B943-A347-7F74EFCA0DB5}"/>
-    <hyperlink ref="B265" r:id="rId243" xr:uid="{6E0EF7A3-7341-284B-A0E3-4539B6EAFAF2}"/>
-    <hyperlink ref="B266" r:id="rId244" xr:uid="{D2D8D64F-E2D3-734E-AD45-3EFB9686555A}"/>
-    <hyperlink ref="B267" r:id="rId245" xr:uid="{04A2904A-73A0-7845-9868-2CCFE359AC68}"/>
-    <hyperlink ref="B268" r:id="rId246" xr:uid="{D3D35835-6BE3-4D41-AF6F-5FE442277A16}"/>
-    <hyperlink ref="B269" r:id="rId247" xr:uid="{F663D0FC-CFF0-BC4F-9D26-48C871A8E9FD}"/>
-    <hyperlink ref="B270" r:id="rId248" xr:uid="{DF544147-DA48-4041-A4E2-4A75106B771A}"/>
-    <hyperlink ref="B271" r:id="rId249" xr:uid="{50E4B716-239E-7946-843D-E8462591D128}"/>
-    <hyperlink ref="B272" r:id="rId250" xr:uid="{D368B3E5-7D12-FD48-AFF7-A4A614108940}"/>
-    <hyperlink ref="B275" r:id="rId251" xr:uid="{D5921FF1-FC1F-CA4B-A24E-AD69E1DEC14C}"/>
-    <hyperlink ref="B276" r:id="rId252" xr:uid="{C931D7E0-E032-7C4B-95F1-735D955FCB51}"/>
-    <hyperlink ref="B277" r:id="rId253" xr:uid="{5FBD4A8F-287C-2C46-9CAB-F7DBA67DEDDA}"/>
-    <hyperlink ref="B278" r:id="rId254" xr:uid="{12966DD6-41DD-A94B-8B2C-0AD7D2AD6FB0}"/>
-    <hyperlink ref="B279" r:id="rId255" xr:uid="{CF720C34-4554-2944-A818-020ABC9BF0F4}"/>
-    <hyperlink ref="B280" r:id="rId256" xr:uid="{75763F2A-16D7-DE43-8189-19623CE26370}"/>
-    <hyperlink ref="B281" r:id="rId257" xr:uid="{9263AA30-472A-0A4D-BADF-96D82BB9BFCC}"/>
-    <hyperlink ref="B282" r:id="rId258" xr:uid="{2EF025C3-75C8-564E-BA8B-708C32B0E602}"/>
-    <hyperlink ref="B283" r:id="rId259" xr:uid="{6BDFDCA9-3421-F24F-8EF2-A72742F0AC21}"/>
-    <hyperlink ref="B284" r:id="rId260" xr:uid="{D8447F99-5FF9-D544-99BB-E9969B4A38D7}"/>
-    <hyperlink ref="B285" r:id="rId261" xr:uid="{1DB7EFDA-6C7D-F546-9EE1-F61ED0F65209}"/>
-    <hyperlink ref="B286" r:id="rId262" xr:uid="{D1505609-27D1-784D-ACF6-AE9D0DA2E1B6}"/>
-    <hyperlink ref="B287" r:id="rId263" xr:uid="{6BFA7B45-17D0-4E49-85DA-23C7255A306D}"/>
-    <hyperlink ref="B288" r:id="rId264" xr:uid="{3324BA4A-30CA-5246-8C3C-6505A6987939}"/>
-    <hyperlink ref="B289" r:id="rId265" xr:uid="{894486AD-2B6D-5740-BCAF-0BA1AFF814B4}"/>
-    <hyperlink ref="B290" r:id="rId266" xr:uid="{C47B203B-8B5A-E740-8C86-0784AD28089E}"/>
-    <hyperlink ref="B291" r:id="rId267" xr:uid="{06DC2E54-7597-AE4D-ACDB-B8883A989A4F}"/>
-    <hyperlink ref="B292" r:id="rId268" xr:uid="{E3384259-7CA7-1C44-A66D-11346EE6742E}"/>
-    <hyperlink ref="B293" r:id="rId269" xr:uid="{A5B77769-38AF-3D47-A76B-311591B57D91}"/>
-    <hyperlink ref="B296" r:id="rId270" xr:uid="{9DB6976A-C646-1341-90E8-3A164521267A}"/>
-    <hyperlink ref="B297" r:id="rId271" xr:uid="{03C291F8-D19A-304B-9EF9-CF71A1F66E49}"/>
-    <hyperlink ref="B298" r:id="rId272" xr:uid="{7536415C-140B-9244-B0B2-23F3ED0B2D80}"/>
-    <hyperlink ref="B299" r:id="rId273" xr:uid="{7DBDA456-8AF6-DD43-9764-17D3959B8E8F}"/>
-    <hyperlink ref="B300" r:id="rId274" xr:uid="{BFC149AB-C15A-B648-9F6A-ECD3890B1918}"/>
-    <hyperlink ref="B301" r:id="rId275" xr:uid="{0482240B-FEE9-F746-8980-52BCB7BBB56E}"/>
-    <hyperlink ref="B302" r:id="rId276" xr:uid="{86D1231A-E7C8-4B45-99ED-2DB0EF71E190}"/>
-    <hyperlink ref="B303" r:id="rId277" xr:uid="{20B7CE89-CB37-0040-989F-C8D1BE2B8782}"/>
-    <hyperlink ref="B304" r:id="rId278" xr:uid="{4C8412C9-A47B-9244-A18B-741516BD1054}"/>
-    <hyperlink ref="B305" r:id="rId279" xr:uid="{511761D9-31CE-0B43-AFFD-C011C27ACC52}"/>
-    <hyperlink ref="B306" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{6905F997-D048-1049-BA27-C48756603D1E}"/>
-    <hyperlink ref="B307" r:id="rId281" xr:uid="{E657AA82-7CFE-DB42-B20F-F63D8C25EAB6}"/>
-    <hyperlink ref="B308" r:id="rId282" xr:uid="{3E505033-58F3-8F4E-AB82-E12DBC226AEA}"/>
-    <hyperlink ref="B309" r:id="rId283" xr:uid="{749599E5-4972-7343-B13B-87E26F837470}"/>
-    <hyperlink ref="B310" r:id="rId284" xr:uid="{12AA88DC-22AB-5A49-B28C-F04C8E35A215}"/>
-    <hyperlink ref="B311" r:id="rId285" xr:uid="{5751F0A7-7D9D-4148-820B-5B9659DFE34F}"/>
-    <hyperlink ref="B312" r:id="rId286" xr:uid="{4CA2DBEE-B161-B84D-B3A9-B8BC1B598AF2}"/>
-    <hyperlink ref="B313" r:id="rId287" xr:uid="{A9C1E578-6594-954C-8785-8902E605FC7A}"/>
-    <hyperlink ref="B314" r:id="rId288" xr:uid="{3D45E9B8-6671-A747-8C18-51CF8883170A}"/>
-    <hyperlink ref="B315" r:id="rId289" xr:uid="{4F5EF748-8CD4-0F47-90CE-3C93755BF63D}"/>
-    <hyperlink ref="B316" r:id="rId290" xr:uid="{44053C08-5050-C84B-B016-069B1EF9A43D}"/>
-    <hyperlink ref="B317" r:id="rId291" xr:uid="{ABF38928-736B-1A49-8B8A-1DCA5AAECB2B}"/>
-    <hyperlink ref="B318" r:id="rId292" xr:uid="{52651FAF-F3DC-E949-8AF8-998B9724B7D1}"/>
-    <hyperlink ref="B319" r:id="rId293" xr:uid="{91C6CCEF-3FF7-2C42-B5A0-8F4A403ED198}"/>
-    <hyperlink ref="B320" r:id="rId294" xr:uid="{15C8AF08-1A79-F949-9BE7-DD240CBD9861}"/>
-    <hyperlink ref="B321" r:id="rId295" xr:uid="{1904F984-5B22-8D46-BC33-3073B390E8F9}"/>
-    <hyperlink ref="B322" r:id="rId296" xr:uid="{A8BFB3A4-426B-E646-BCF0-FE19C8CD07A9}"/>
-    <hyperlink ref="B323" r:id="rId297" xr:uid="{FBBA29BB-885B-744A-A644-58EDCA7B140A}"/>
-    <hyperlink ref="B324" r:id="rId298" xr:uid="{75411687-6884-AC42-8B4A-1348C4837365}"/>
-    <hyperlink ref="B325" r:id="rId299" xr:uid="{A89ED8DF-F678-FE43-808C-C190721379BF}"/>
-    <hyperlink ref="B326" r:id="rId300" xr:uid="{1516834D-F3B2-1743-8811-263E11BBDEF8}"/>
-    <hyperlink ref="B327" r:id="rId301" xr:uid="{1659AB91-08CA-E44D-988D-E9D9A746D406}"/>
-    <hyperlink ref="B328" r:id="rId302" xr:uid="{E844BC1D-9713-9F4D-B0A4-1124A9952D14}"/>
-    <hyperlink ref="B329" r:id="rId303" xr:uid="{DCE2AAEF-8D8E-1843-BFE9-E9B7E13854EB}"/>
-    <hyperlink ref="B330" r:id="rId304" xr:uid="{836B3BF0-7711-7D41-9E72-914C1871397F}"/>
-    <hyperlink ref="B331" r:id="rId305" xr:uid="{F450CF9B-CA59-1443-8163-13F1121DCF12}"/>
-    <hyperlink ref="B332" r:id="rId306" xr:uid="{1539C3E8-4854-3C4F-A7B3-55BF931F1E2A}"/>
-    <hyperlink ref="B333" r:id="rId307" xr:uid="{04F1FC5F-5DA1-0144-962D-B38C1C41F0F4}"/>
-    <hyperlink ref="B336" r:id="rId308" xr:uid="{B21618F4-70E2-C549-80B7-7CF915679E0A}"/>
-    <hyperlink ref="B337" r:id="rId309" xr:uid="{EEDFBF11-C1E4-0847-9D56-94A72D97AEE7}"/>
-    <hyperlink ref="B338" r:id="rId310" xr:uid="{F5C0EDF1-7EAC-8849-8D27-C3389913BFC6}"/>
-    <hyperlink ref="B339" r:id="rId311" xr:uid="{50175B29-124F-4E4E-8E98-961BD3320359}"/>
-    <hyperlink ref="B340" r:id="rId312" xr:uid="{1BE23822-8512-014F-9154-F6EDA4FC8428}"/>
-    <hyperlink ref="B341" r:id="rId313" xr:uid="{38EC228E-ABFF-3542-9CFB-3DDFC628E9D0}"/>
-    <hyperlink ref="B342" r:id="rId314" xr:uid="{73F240F8-C469-454E-BA5C-CFF2F7A7A5F6}"/>
-    <hyperlink ref="B343" r:id="rId315" xr:uid="{3BBD1BAC-68C7-A94A-9063-AF62B5C837FD}"/>
-    <hyperlink ref="B344" r:id="rId316" xr:uid="{F9751D9B-2689-E24B-9FC3-CA32FE888708}"/>
-    <hyperlink ref="B345" r:id="rId317" xr:uid="{73C61D6A-D97C-B944-8B27-BB91564AB0D7}"/>
-    <hyperlink ref="B346" r:id="rId318" xr:uid="{936E077C-C016-A04F-895A-782D6D9D9433}"/>
-    <hyperlink ref="B347" r:id="rId319" xr:uid="{5454A2A1-6607-BE48-9215-CB8965EC3568}"/>
-    <hyperlink ref="B348" r:id="rId320" xr:uid="{FC1EAA10-F7ED-6B42-A79B-3D8B44E2C8B3}"/>
-    <hyperlink ref="B349" r:id="rId321" xr:uid="{FDB7F712-4A42-1048-8929-A1E752B07C6A}"/>
-    <hyperlink ref="B350" r:id="rId322" xr:uid="{AF3ACA60-0B0E-E146-B51F-A2CD05EB6549}"/>
-    <hyperlink ref="B351" r:id="rId323" xr:uid="{BB63E040-7A1A-E046-9BDD-9CBD1DA89DE9}"/>
-    <hyperlink ref="B352" r:id="rId324" xr:uid="{9AF8FD93-CCC9-D540-AE9A-00583F309649}"/>
-    <hyperlink ref="B353" r:id="rId325" xr:uid="{66A746A0-71FE-E546-92B7-D1C3D582E067}"/>
-    <hyperlink ref="B357" r:id="rId326" xr:uid="{BD79CCE1-5315-3944-9F9B-618615EC4583}"/>
-    <hyperlink ref="B358" r:id="rId327" xr:uid="{A5068A51-C961-6847-BB27-40A850B6D393}"/>
-    <hyperlink ref="B359" r:id="rId328" xr:uid="{6B8D36F0-E796-B944-A456-E8A9E2EE0BDB}"/>
-    <hyperlink ref="B360" r:id="rId329" xr:uid="{776652B7-2C11-4641-BF6A-EABEEB9B55AB}"/>
-    <hyperlink ref="B361" r:id="rId330" xr:uid="{95C6B35D-712A-2343-B790-236B55C5EC49}"/>
-    <hyperlink ref="B362" r:id="rId331" xr:uid="{4ED53872-1FE9-F140-AA35-F228F762880B}"/>
-    <hyperlink ref="B363" r:id="rId332" xr:uid="{6D5E6A28-85AA-BF4C-B2BD-9378D6E28EC7}"/>
-    <hyperlink ref="B364" r:id="rId333" xr:uid="{BCAD1ECB-15EE-CF49-878E-AA682DE3AC22}"/>
-    <hyperlink ref="B365" r:id="rId334" xr:uid="{C85468B5-25E9-E446-808E-72CFE911F0C2}"/>
-    <hyperlink ref="B366" r:id="rId335" xr:uid="{9503AECA-1A6A-9640-A04C-4CEAA2304448}"/>
-    <hyperlink ref="B367" r:id="rId336" xr:uid="{74211516-06B0-AA45-845B-52C8202751DA}"/>
-    <hyperlink ref="B368" r:id="rId337" xr:uid="{02C696BC-4B91-9444-900F-9CD68E409ABC}"/>
-    <hyperlink ref="B369" r:id="rId338" xr:uid="{04646C45-4118-374C-839D-94D31D534FAC}"/>
-    <hyperlink ref="B370" r:id="rId339" xr:uid="{F90BCCAE-8596-FC4D-BDD7-774392C596DF}"/>
-    <hyperlink ref="B371" r:id="rId340" xr:uid="{65230925-36EC-8A4B-8E46-6350B9BC0F95}"/>
-    <hyperlink ref="B372" r:id="rId341" xr:uid="{E91B8177-0C7A-1F40-BD34-4CC60F03B84F}"/>
-    <hyperlink ref="B373" r:id="rId342" xr:uid="{E8CBFD60-7335-0B4D-9FF5-99B4A8DC551D}"/>
-    <hyperlink ref="B374" r:id="rId343" xr:uid="{A35F55D4-9B87-C745-94DB-E7D820193C30}"/>
-    <hyperlink ref="B375" r:id="rId344" xr:uid="{6461A29F-D404-334F-B13F-296B4CA5E8A4}"/>
-    <hyperlink ref="B376" r:id="rId345" xr:uid="{FA9B4BE7-85CC-B24F-9461-5E9B42DDD824}"/>
-    <hyperlink ref="B377" r:id="rId346" xr:uid="{A75ACEA2-CDF6-A147-8540-A6DF55B15F45}"/>
-    <hyperlink ref="B378" r:id="rId347" xr:uid="{62FF87E2-E658-AB4D-AC57-7BCF9D49516E}"/>
-    <hyperlink ref="B379" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
-    <hyperlink ref="B380" r:id="rId349" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
-    <hyperlink ref="B381" r:id="rId350" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
-    <hyperlink ref="B382" r:id="rId351" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
-    <hyperlink ref="B383" r:id="rId352" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
-    <hyperlink ref="B384" r:id="rId353" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
-    <hyperlink ref="B385" r:id="rId354" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
-    <hyperlink ref="B386" r:id="rId355" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
-    <hyperlink ref="B387" r:id="rId356" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
-    <hyperlink ref="B388" r:id="rId357" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
-    <hyperlink ref="B389" r:id="rId358" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
-    <hyperlink ref="B390" r:id="rId359" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
-    <hyperlink ref="B391" r:id="rId360" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
-    <hyperlink ref="B392" r:id="rId361" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
-    <hyperlink ref="B393" r:id="rId362" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
-    <hyperlink ref="B394" r:id="rId363" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
-    <hyperlink ref="B396" r:id="rId364" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
-    <hyperlink ref="B395" r:id="rId365" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
-    <hyperlink ref="B397" r:id="rId366" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
-    <hyperlink ref="B398" r:id="rId367" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
-    <hyperlink ref="B399" r:id="rId368" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
-    <hyperlink ref="B402" r:id="rId369" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
-    <hyperlink ref="B403" r:id="rId370" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
-    <hyperlink ref="B404" r:id="rId371" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
-    <hyperlink ref="B405" r:id="rId372" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
-    <hyperlink ref="B406" r:id="rId373" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
-    <hyperlink ref="B407" r:id="rId374" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
-    <hyperlink ref="B410" r:id="rId375" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
-    <hyperlink ref="B411" r:id="rId376" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
-    <hyperlink ref="B412" r:id="rId377" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
-    <hyperlink ref="B413" r:id="rId378" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
-    <hyperlink ref="B414" r:id="rId379" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
-    <hyperlink ref="B415" r:id="rId380" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
-    <hyperlink ref="B416" r:id="rId381" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
-    <hyperlink ref="B417" r:id="rId382" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
-    <hyperlink ref="B418" r:id="rId383" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
-    <hyperlink ref="B419" r:id="rId384" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
-    <hyperlink ref="B420" r:id="rId385" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
-    <hyperlink ref="B421" r:id="rId386" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
-    <hyperlink ref="B422" r:id="rId387" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
-    <hyperlink ref="B423" r:id="rId388" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
-    <hyperlink ref="B424" r:id="rId389" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
-    <hyperlink ref="B425" r:id="rId390" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
-    <hyperlink ref="B426" r:id="rId391" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
-    <hyperlink ref="B427" r:id="rId392" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
-    <hyperlink ref="B428" r:id="rId393" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
-    <hyperlink ref="B429" r:id="rId394" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
-    <hyperlink ref="B430" r:id="rId395" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
-    <hyperlink ref="B431" r:id="rId396" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
-    <hyperlink ref="B432" r:id="rId397" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
-    <hyperlink ref="B433" r:id="rId398" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
-    <hyperlink ref="B434" r:id="rId399" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
-    <hyperlink ref="B435" r:id="rId400" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
-    <hyperlink ref="B436" r:id="rId401" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
-    <hyperlink ref="B437" r:id="rId402" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
-    <hyperlink ref="B438" r:id="rId403" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
-    <hyperlink ref="B439" r:id="rId404" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
-    <hyperlink ref="B440" r:id="rId405" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
-    <hyperlink ref="B441" r:id="rId406" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
-    <hyperlink ref="B442" r:id="rId407" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
-    <hyperlink ref="B443" r:id="rId408" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
-    <hyperlink ref="B444" r:id="rId409" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
-    <hyperlink ref="B445" r:id="rId410" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
-    <hyperlink ref="B446" r:id="rId411" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
-    <hyperlink ref="B447" r:id="rId412" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
-    <hyperlink ref="B448" r:id="rId413" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
-    <hyperlink ref="B449" r:id="rId414" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
-    <hyperlink ref="B451" r:id="rId415" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
-    <hyperlink ref="B450" r:id="rId416" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
-    <hyperlink ref="B452" r:id="rId417" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
-    <hyperlink ref="B453" r:id="rId418" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
-    <hyperlink ref="B454" r:id="rId419" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
-    <hyperlink ref="B455" r:id="rId420" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
-    <hyperlink ref="B456" r:id="rId421" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
-    <hyperlink ref="B457" r:id="rId422" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
-    <hyperlink ref="B458" r:id="rId423" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
-    <hyperlink ref="B459" r:id="rId424" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
-    <hyperlink ref="B460" r:id="rId425" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
-    <hyperlink ref="B461" r:id="rId426" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
-    <hyperlink ref="B462" r:id="rId427" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
-    <hyperlink ref="B469" r:id="rId428" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
-    <hyperlink ref="B468" r:id="rId429" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
-    <hyperlink ref="B467" r:id="rId430" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
-    <hyperlink ref="B466" r:id="rId431" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
-    <hyperlink ref="B465" r:id="rId432" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
-    <hyperlink ref="B464" r:id="rId433" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
-    <hyperlink ref="B463" r:id="rId434" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
-    <hyperlink ref="B472" r:id="rId435" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
-    <hyperlink ref="B473" r:id="rId436" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
-    <hyperlink ref="B474" r:id="rId437" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
-    <hyperlink ref="B475" r:id="rId438" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
-    <hyperlink ref="B476" r:id="rId439" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
-    <hyperlink ref="B477" r:id="rId440" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
-    <hyperlink ref="B478" r:id="rId441" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="B481" r:id="rId442" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
-    <hyperlink ref="B479" r:id="rId443" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
-    <hyperlink ref="B480" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
-    <hyperlink ref="B356" r:id="rId445" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
-    <hyperlink ref="B2" r:id="rId446" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
+    <hyperlink ref="B96" r:id="rId77" xr:uid="{F152A9AF-5CBA-EC44-A9CF-07AB481435AB}"/>
+    <hyperlink ref="B97" r:id="rId78" xr:uid="{346CA74F-60B7-0A4B-A612-9184D4DCFF62}"/>
+    <hyperlink ref="B98" r:id="rId79" xr:uid="{8C653CB1-4954-754F-8D46-F09141A2FCDB}"/>
+    <hyperlink ref="B101" r:id="rId80" xr:uid="{5989F693-2A61-A346-8395-8674307A4CC2}"/>
+    <hyperlink ref="B102" r:id="rId81" xr:uid="{3AD10C9E-4F6D-DE48-92F3-531A586520C6}"/>
+    <hyperlink ref="B103" r:id="rId82" xr:uid="{4FA217C0-A1F3-904E-8FEA-EA4941273A67}"/>
+    <hyperlink ref="B104" r:id="rId83" xr:uid="{A297BBC0-FA0D-2D46-9C49-3932193EF1D3}"/>
+    <hyperlink ref="B106" r:id="rId84" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance." xr:uid="{DCD751DE-E440-F346-B6FD-CBD072217214}"/>
+    <hyperlink ref="B107" r:id="rId85" xr:uid="{B2FD38B9-1E2B-8140-8291-F45734C98145}"/>
+    <hyperlink ref="B108" r:id="rId86" xr:uid="{C76888B3-18AC-9B48-9E2A-64A7DF0902B7}"/>
+    <hyperlink ref="B109" r:id="rId87" xr:uid="{18A79860-6C9E-A941-8D6C-360B9913E941}"/>
+    <hyperlink ref="B110" r:id="rId88" xr:uid="{C0DDFD68-CBC1-0F4A-AF40-ACF36BBC8453}"/>
+    <hyperlink ref="B111" r:id="rId89" xr:uid="{3E0BF737-E42E-C946-B32C-06882E0BA6FF}"/>
+    <hyperlink ref="B113" r:id="rId90" xr:uid="{862F9782-C57B-2848-A2D9-EB7B52FB7EC7}"/>
+    <hyperlink ref="B114" r:id="rId91" xr:uid="{230D7A6A-D2C5-C140-9A65-B1F407D22062}"/>
+    <hyperlink ref="B115" r:id="rId92" xr:uid="{BDC2BA28-4562-984E-8282-1126BF952EAF}"/>
+    <hyperlink ref="B116" r:id="rId93" xr:uid="{B53A5F28-6DED-3D47-8679-F78D3DDEFF01}"/>
+    <hyperlink ref="B117" r:id="rId94" xr:uid="{C57D0CC7-DA2F-0948-9BCE-F19C20C7D981}"/>
+    <hyperlink ref="B118" r:id="rId95" xr:uid="{117878E5-B8C8-254B-8ED6-014B4B7A8126}"/>
+    <hyperlink ref="B119" r:id="rId96" xr:uid="{B7CC0756-74F2-D54D-BDEE-9DA394DD7168}"/>
+    <hyperlink ref="B120" r:id="rId97" xr:uid="{837EF472-CCC2-CF47-A8A8-238E56F722CE}"/>
+    <hyperlink ref="B121" r:id="rId98" xr:uid="{3608F267-6AA0-624B-B243-7DDD317E9F08}"/>
+    <hyperlink ref="B122" r:id="rId99" xr:uid="{0B6123E6-0472-374B-ACA7-6914CD7918E8}"/>
+    <hyperlink ref="B123" r:id="rId100" xr:uid="{D3971CEB-C53E-B04B-9C32-1803182B5DC5}"/>
+    <hyperlink ref="B124" r:id="rId101" xr:uid="{7CF5013A-643E-1643-93A1-A2F1500D2A23}"/>
+    <hyperlink ref="B125" r:id="rId102" xr:uid="{2A6BE7E5-D818-6843-8C3E-99EA2BFE0FB2}"/>
+    <hyperlink ref="B126" r:id="rId103" xr:uid="{E718F544-96DF-A04E-8DFB-7639DA3EA57C}"/>
+    <hyperlink ref="B127" r:id="rId104" xr:uid="{B0C2F065-424A-7345-A864-346ECD98D749}"/>
+    <hyperlink ref="B128" r:id="rId105" xr:uid="{B4E26955-5C3F-804E-B19A-11260310AFB3}"/>
+    <hyperlink ref="B129" r:id="rId106" xr:uid="{6F299BB5-8E82-0240-A9A3-6829CE3ABCBF}"/>
+    <hyperlink ref="B130" r:id="rId107" xr:uid="{A42CA32F-2196-1840-A53D-E5073237C68D}"/>
+    <hyperlink ref="B131" r:id="rId108" xr:uid="{7ECF6EF4-962E-4642-9B1C-C3B70674793E}"/>
+    <hyperlink ref="B132" r:id="rId109" xr:uid="{2A109178-6B60-164E-9D25-42B3282137E3}"/>
+    <hyperlink ref="B133" r:id="rId110" xr:uid="{B3D38BD0-A6A1-8D41-8405-45E1BEEEEF06}"/>
+    <hyperlink ref="B134" r:id="rId111" xr:uid="{A1C26612-D040-2A41-A6A6-A8F2490C0A43}"/>
+    <hyperlink ref="B135" r:id="rId112" xr:uid="{C476E807-64CB-F44A-A23D-D21EBF6D001D}"/>
+    <hyperlink ref="B136" r:id="rId113" xr:uid="{9A414D55-D4A1-F147-9207-61B597D57136}"/>
+    <hyperlink ref="B105" r:id="rId114" xr:uid="{18B028A7-9B6F-D841-8548-924D70530779}"/>
+    <hyperlink ref="B112" r:id="rId115" xr:uid="{6D3E75EF-733F-7A4B-81C8-AEF6CB6335F0}"/>
+    <hyperlink ref="B139" r:id="rId116" xr:uid="{C9EB2682-BE0B-934B-B0B4-1DD1A1502647}"/>
+    <hyperlink ref="B140" r:id="rId117" xr:uid="{2992FED9-2B78-A342-92AA-E7C0F882FF17}"/>
+    <hyperlink ref="B141" r:id="rId118" xr:uid="{0084DA6F-EC84-BD48-BDA8-EBACA3BB3B3E}"/>
+    <hyperlink ref="B142" r:id="rId119" xr:uid="{30F2D415-4B2C-384C-8EAE-2CC71CB518E2}"/>
+    <hyperlink ref="B143" r:id="rId120" xr:uid="{40734C88-7C5B-9747-86D1-03463D9AD41A}"/>
+    <hyperlink ref="B144" r:id="rId121" xr:uid="{1040D22F-6729-104A-A229-CBDCED93024A}"/>
+    <hyperlink ref="B145" r:id="rId122" xr:uid="{E131FE61-FABF-8E4B-8EF0-F68379D8F836}"/>
+    <hyperlink ref="B146" r:id="rId123" xr:uid="{B2129272-1351-3745-883B-E6A7115450C8}"/>
+    <hyperlink ref="B147" r:id="rId124" xr:uid="{C8B2DEF0-2B69-C84E-8013-0B6F03FFC250}"/>
+    <hyperlink ref="B148" r:id="rId125" xr:uid="{536AC5CF-712F-BF48-94A9-D0E7DC013020}"/>
+    <hyperlink ref="B149" r:id="rId126" xr:uid="{2DABC9C7-43D4-1249-AF9B-5FA4552611CB}"/>
+    <hyperlink ref="B150" r:id="rId127" xr:uid="{DA62E73A-B495-F94A-BECE-D42E4CBF074A}"/>
+    <hyperlink ref="B151" r:id="rId128" xr:uid="{7F5E6966-850D-4F49-B2A5-678365713F28}"/>
+    <hyperlink ref="B152" r:id="rId129" xr:uid="{E9C4286D-8493-9A47-8B8C-09583FA72B70}"/>
+    <hyperlink ref="B153" r:id="rId130" xr:uid="{9EB0123C-84AE-1C4D-BA1A-C28CFB8EFB89}"/>
+    <hyperlink ref="B154" r:id="rId131" xr:uid="{9D11FED4-328F-674E-889D-EC781DD1D791}"/>
+    <hyperlink ref="B155" r:id="rId132" xr:uid="{48AE72DB-397B-464D-88AD-B8058ED29CC1}"/>
+    <hyperlink ref="B156" r:id="rId133" xr:uid="{152D50E9-7448-F542-AC66-05D0AE66664C}"/>
+    <hyperlink ref="B157" r:id="rId134" xr:uid="{34E6AF1B-5FB1-3A4B-8938-1DCF80831DC2}"/>
+    <hyperlink ref="B158" r:id="rId135" xr:uid="{E7F8B7CA-49F4-1946-91EE-E7582BE4E5DA}"/>
+    <hyperlink ref="B159" r:id="rId136" xr:uid="{3590A994-B7A2-C14D-9BF8-7AC8FE9E7F0F}"/>
+    <hyperlink ref="B160" r:id="rId137" xr:uid="{0AAA4B0C-4921-C34D-B41E-D702FA860892}"/>
+    <hyperlink ref="B161" r:id="rId138" xr:uid="{5973FCA4-AE32-5248-A6ED-2694367332F1}"/>
+    <hyperlink ref="B162" r:id="rId139" xr:uid="{4C0F816E-F043-0C47-BF16-1CDAD88D2FF1}"/>
+    <hyperlink ref="B163" r:id="rId140" xr:uid="{A8E4C654-D0BD-8945-9F5C-B09F7BC114BE}"/>
+    <hyperlink ref="B166" r:id="rId141" xr:uid="{E3825C15-10BB-E24F-B229-983F651DA942}"/>
+    <hyperlink ref="B167" r:id="rId142" xr:uid="{46ECFC31-388C-6241-8FFE-DED6F2FC794A}"/>
+    <hyperlink ref="B168" r:id="rId143" xr:uid="{589E024D-3FE1-1048-890C-88289733F233}"/>
+    <hyperlink ref="B169" r:id="rId144" xr:uid="{CDA28F7A-7FC5-F74D-B27E-A6E0161D41D5}"/>
+    <hyperlink ref="B170" r:id="rId145" xr:uid="{DA6A0D92-DCEB-DA4F-8BBA-10FCD092838F}"/>
+    <hyperlink ref="B171" r:id="rId146" xr:uid="{955769DB-3256-254B-90DE-E1E01B272F8A}"/>
+    <hyperlink ref="B172" r:id="rId147" xr:uid="{DED7AC9B-40D7-0545-9D6F-6CD4F5FFE4C6}"/>
+    <hyperlink ref="B173" r:id="rId148" xr:uid="{6947A4E1-B6AA-6D4F-A6D8-8FA74FD02887}"/>
+    <hyperlink ref="B174" r:id="rId149" xr:uid="{EABF2012-5A90-0C4E-86F6-FDB5FA7770BE}"/>
+    <hyperlink ref="B177" r:id="rId150" xr:uid="{7F44CFE0-9ED1-A44D-B9EF-CF87BEB644FC}"/>
+    <hyperlink ref="B178" r:id="rId151" xr:uid="{CF6E0CF6-7A93-D84A-9CE0-5BDD51767416}"/>
+    <hyperlink ref="B179" r:id="rId152" xr:uid="{EFF8F154-60B8-B84B-84CA-32756BD6430F}"/>
+    <hyperlink ref="B180" r:id="rId153" xr:uid="{C8A3094E-E11B-2543-B05E-1D07048B2EBA}"/>
+    <hyperlink ref="B181" r:id="rId154" xr:uid="{9961E5F5-B5C6-0C4D-A1D0-D04D2A5D7DFD}"/>
+    <hyperlink ref="B182" r:id="rId155" xr:uid="{44E289EC-47DD-D94D-88C1-CB2F59C6C16A}"/>
+    <hyperlink ref="B183" r:id="rId156" xr:uid="{4161FC70-DD6D-684B-898A-A4711596B2D5}"/>
+    <hyperlink ref="B184" r:id="rId157" xr:uid="{B9CBE387-8E9A-ED48-8310-CF7D34FA690C}"/>
+    <hyperlink ref="B185" r:id="rId158" xr:uid="{5398097B-24FF-9543-8F02-33CE2860F1F7}"/>
+    <hyperlink ref="B186" r:id="rId159" xr:uid="{3B1FC30B-30C8-7B48-AF94-A81FB513F24F}"/>
+    <hyperlink ref="B187" r:id="rId160" xr:uid="{32B750D0-D7F2-694D-AB9B-25AFAFAFF17F}"/>
+    <hyperlink ref="B188" r:id="rId161" xr:uid="{400689DD-8E95-024E-976B-AACD8ED4E1A6}"/>
+    <hyperlink ref="B189" r:id="rId162" xr:uid="{28753DDE-E047-5D40-A30B-1103BE6DA08F}"/>
+    <hyperlink ref="B190" r:id="rId163" xr:uid="{6C5AA6CB-3D93-0740-AEED-9E6C218CF6CB}"/>
+    <hyperlink ref="B191" r:id="rId164" xr:uid="{03EAA2B9-D8B8-D642-BF24-380596D26B2E}"/>
+    <hyperlink ref="B192" r:id="rId165" xr:uid="{8C1719B4-37CC-484E-BDCE-A4272C07F91B}"/>
+    <hyperlink ref="B193" r:id="rId166" xr:uid="{6C198DA2-BB98-F940-8EF6-2FC8B7AE577A}"/>
+    <hyperlink ref="B194" r:id="rId167" xr:uid="{AB0EA311-A446-D046-A0EC-290B42068328}"/>
+    <hyperlink ref="B195" r:id="rId168" xr:uid="{DB913045-B9F6-6549-AA09-22B0CC5FDD21}"/>
+    <hyperlink ref="B196" r:id="rId169" xr:uid="{806469FD-617A-7445-AAB5-FB2FD2ED24EA}"/>
+    <hyperlink ref="B197" r:id="rId170" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{1A10544E-58CF-D04D-9FAF-2FEC6DB2B5D4}"/>
+    <hyperlink ref="B198" r:id="rId171" xr:uid="{5A0B6645-89FD-E044-A706-9FB890274C3C}"/>
+    <hyperlink ref="B199" r:id="rId172" xr:uid="{B42A3009-E8EB-EE44-885F-6699C17A0E0B}"/>
+    <hyperlink ref="B200" r:id="rId173" xr:uid="{ED3E48AB-E25B-3744-B024-E97B2A319B46}"/>
+    <hyperlink ref="B201" r:id="rId174" xr:uid="{C75D20A3-CBAE-2649-A3EE-E49177CFA343}"/>
+    <hyperlink ref="B202" r:id="rId175" xr:uid="{3863CA1B-D43E-1144-91A9-17C2DCF52A64}"/>
+    <hyperlink ref="B203" r:id="rId176" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{E9AF434E-4CAA-5D49-8AD3-889CDE2913D9}"/>
+    <hyperlink ref="B204" r:id="rId177" xr:uid="{1A0568E5-3A11-7F47-8001-82B05D7C2339}"/>
+    <hyperlink ref="B205" r:id="rId178" xr:uid="{F62B8AE4-9C4F-9544-8861-CD733C12F79E}"/>
+    <hyperlink ref="B206" r:id="rId179" xr:uid="{0F6A542C-44C9-5A4C-90BF-BC8C239877D2}"/>
+    <hyperlink ref="B207" r:id="rId180" xr:uid="{3ED28203-B1B5-4E46-AAF3-779EDD4AC03F}"/>
+    <hyperlink ref="B208" r:id="rId181" xr:uid="{4338B305-B52F-5540-9B51-B938FC6803A2}"/>
+    <hyperlink ref="B209" r:id="rId182" xr:uid="{DDEEED0F-A939-1E4F-B2FA-AD391A4A2874}"/>
+    <hyperlink ref="B210" r:id="rId183" xr:uid="{C2F20589-AD81-654C-94E5-E5B6C9FE27F6}"/>
+    <hyperlink ref="B211" r:id="rId184" xr:uid="{BBEB9DAC-E4AE-C04F-AA15-6356AFC57FDE}"/>
+    <hyperlink ref="B214" r:id="rId185" xr:uid="{6316566D-A10A-F849-9F25-B9ED4DA12BC7}"/>
+    <hyperlink ref="B215" r:id="rId186" xr:uid="{9D4DD895-FBA6-C849-A5BF-3B30755BD9C9}"/>
+    <hyperlink ref="B216" r:id="rId187" xr:uid="{475996DA-632A-BE49-AEA1-D4189FD614A1}"/>
+    <hyperlink ref="B217" r:id="rId188" xr:uid="{88E0C858-8468-884F-BB71-F6F176BD5FC2}"/>
+    <hyperlink ref="B218" r:id="rId189" xr:uid="{C1C5C8D0-7A06-3D4A-A85A-AAACC1B418C9}"/>
+    <hyperlink ref="B219" r:id="rId190" xr:uid="{D525D4B1-2857-1543-8CD9-196728321203}"/>
+    <hyperlink ref="B220" r:id="rId191" xr:uid="{51E3AB9B-04B2-C041-A2B3-37E3EB18013A}"/>
+    <hyperlink ref="B221" r:id="rId192" xr:uid="{7F7F0C9A-57B9-314F-959A-B8ACAFA5FD13}"/>
+    <hyperlink ref="B222" r:id="rId193" xr:uid="{3B029785-83B4-6140-8B70-CD892CFC87F6}"/>
+    <hyperlink ref="B223" r:id="rId194" xr:uid="{B0A390E6-D860-9F4E-B021-68949FE712F3}"/>
+    <hyperlink ref="B224" r:id="rId195" xr:uid="{49E9953D-52F6-BF47-8AAA-8E456F55576B}"/>
+    <hyperlink ref="B225" r:id="rId196" xr:uid="{9B812470-F419-A54E-8365-06A9B8864A30}"/>
+    <hyperlink ref="B226" r:id="rId197" xr:uid="{B6FB4107-1933-6D45-9EF4-4474E06CBE9D}"/>
+    <hyperlink ref="B227" r:id="rId198" xr:uid="{0F7C1D92-7BCB-D14D-A658-9599984E04E4}"/>
+    <hyperlink ref="B228" r:id="rId199" xr:uid="{6810428F-0A78-964C-A8C8-E1CD2E7C405D}"/>
+    <hyperlink ref="B229" r:id="rId200" xr:uid="{B40209F2-0D6E-364F-8AF6-F1D182509314}"/>
+    <hyperlink ref="B230" r:id="rId201" xr:uid="{96C53FA9-9FD3-2D4F-B292-3C9DEDFA806E}"/>
+    <hyperlink ref="B231" r:id="rId202" xr:uid="{918B420D-3678-FD46-9463-595E8ACC39E1}"/>
+    <hyperlink ref="B232" r:id="rId203" xr:uid="{851A7153-3B54-0E4A-A0A0-FCEB091AFE70}"/>
+    <hyperlink ref="B233" r:id="rId204" xr:uid="{C03AE9F8-09AE-C640-81A7-033BB06FB6AD}"/>
+    <hyperlink ref="B234" r:id="rId205" xr:uid="{35140DEB-52D2-4342-88D2-22BA061E5B48}"/>
+    <hyperlink ref="B235" r:id="rId206" xr:uid="{9714BC0B-3373-934C-B7A1-599F74F4FB9D}"/>
+    <hyperlink ref="B238" r:id="rId207" xr:uid="{5CB435B2-7FD2-1D44-9872-22B6A1EDC02B}"/>
+    <hyperlink ref="B239" r:id="rId208" xr:uid="{722D1D95-896B-4642-BABD-31DEDD237B49}"/>
+    <hyperlink ref="B240" r:id="rId209" xr:uid="{D686D1DC-13D6-284C-B606-E087FAF47399}"/>
+    <hyperlink ref="B241" r:id="rId210" xr:uid="{D22C2394-C3CB-8F4F-A010-2B13C8C84D1A}"/>
+    <hyperlink ref="B242" r:id="rId211" xr:uid="{3AE2F800-B66F-1A41-893B-978F6875FDC8}"/>
+    <hyperlink ref="B243" r:id="rId212" xr:uid="{2C939BDE-5298-5541-837B-8C59D53A33C1}"/>
+    <hyperlink ref="B244" r:id="rId213" xr:uid="{691C9BD8-69D3-DA4B-AEB6-AF827B4ACA9F}"/>
+    <hyperlink ref="B245" r:id="rId214" xr:uid="{B6891E82-7C4D-424D-9219-3C9FD08E0053}"/>
+    <hyperlink ref="B246" r:id="rId215" xr:uid="{67A1AE98-62D2-644D-AC13-6CD76CF53CC0}"/>
+    <hyperlink ref="B247" r:id="rId216" xr:uid="{B59D4881-2A82-8F4D-B151-1E796C4923C8}"/>
+    <hyperlink ref="B248" r:id="rId217" xr:uid="{B3CBD023-5EFD-6048-9B3F-89F0C65CBBF5}"/>
+    <hyperlink ref="B249" r:id="rId218" xr:uid="{53EC42C4-22F7-0445-A0AC-7275A59A2672}"/>
+    <hyperlink ref="B250" r:id="rId219" xr:uid="{A29575F3-CB24-5B4B-9538-D5212B2DC28B}"/>
+    <hyperlink ref="B251" r:id="rId220" xr:uid="{353A44DD-9E30-8F48-8E2B-8DAA07550470}"/>
+    <hyperlink ref="B252" r:id="rId221" xr:uid="{32AC291D-95A5-BE49-88E0-02677BF39CAC}"/>
+    <hyperlink ref="B253" r:id="rId222" xr:uid="{A84F22FF-AD10-A546-8998-B066C0EB2D5A}"/>
+    <hyperlink ref="B254" r:id="rId223" xr:uid="{4C5CAF84-9B94-FC44-8C6C-B3CC7257C1DB}"/>
+    <hyperlink ref="B255" r:id="rId224" xr:uid="{5DA775E2-C516-3B47-8C82-3CEE7CC0BDF9}"/>
+    <hyperlink ref="B256" r:id="rId225" xr:uid="{00B6AE5C-EF3F-0747-A280-3BF055362B4F}"/>
+    <hyperlink ref="B257" r:id="rId226" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{BCBD0A7E-F3D0-E840-9375-AFD37C5CD41A}"/>
+    <hyperlink ref="B258" r:id="rId227" xr:uid="{47ABDDDB-F95F-8049-9FB3-1E71A7376DDE}"/>
+    <hyperlink ref="B259" r:id="rId228" xr:uid="{70BADFC9-7399-234D-99F6-4C5F02397C26}"/>
+    <hyperlink ref="B260" r:id="rId229" xr:uid="{63348580-70EF-EC47-BF49-8ECE9560D54E}"/>
+    <hyperlink ref="B261" r:id="rId230" xr:uid="{D5BD96B3-9EAB-1B47-AC87-5C47F6AD7F40}"/>
+    <hyperlink ref="B262" r:id="rId231" xr:uid="{74791141-3FB8-7540-B45B-9541AF0AE371}"/>
+    <hyperlink ref="B263" r:id="rId232" xr:uid="{88D53CD6-262A-7247-8E58-FE9FFF7ECC40}"/>
+    <hyperlink ref="B264" r:id="rId233" xr:uid="{4338A14D-4F7D-B943-A347-7F74EFCA0DB5}"/>
+    <hyperlink ref="B265" r:id="rId234" xr:uid="{6E0EF7A3-7341-284B-A0E3-4539B6EAFAF2}"/>
+    <hyperlink ref="B266" r:id="rId235" xr:uid="{D2D8D64F-E2D3-734E-AD45-3EFB9686555A}"/>
+    <hyperlink ref="B267" r:id="rId236" xr:uid="{04A2904A-73A0-7845-9868-2CCFE359AC68}"/>
+    <hyperlink ref="B268" r:id="rId237" xr:uid="{D3D35835-6BE3-4D41-AF6F-5FE442277A16}"/>
+    <hyperlink ref="B269" r:id="rId238" xr:uid="{F663D0FC-CFF0-BC4F-9D26-48C871A8E9FD}"/>
+    <hyperlink ref="B270" r:id="rId239" xr:uid="{DF544147-DA48-4041-A4E2-4A75106B771A}"/>
+    <hyperlink ref="B271" r:id="rId240" xr:uid="{50E4B716-239E-7946-843D-E8462591D128}"/>
+    <hyperlink ref="B272" r:id="rId241" xr:uid="{D368B3E5-7D12-FD48-AFF7-A4A614108940}"/>
+    <hyperlink ref="B275" r:id="rId242" xr:uid="{D5921FF1-FC1F-CA4B-A24E-AD69E1DEC14C}"/>
+    <hyperlink ref="B276" r:id="rId243" xr:uid="{C931D7E0-E032-7C4B-95F1-735D955FCB51}"/>
+    <hyperlink ref="B277" r:id="rId244" xr:uid="{5FBD4A8F-287C-2C46-9CAB-F7DBA67DEDDA}"/>
+    <hyperlink ref="B278" r:id="rId245" xr:uid="{12966DD6-41DD-A94B-8B2C-0AD7D2AD6FB0}"/>
+    <hyperlink ref="B279" r:id="rId246" xr:uid="{CF720C34-4554-2944-A818-020ABC9BF0F4}"/>
+    <hyperlink ref="B280" r:id="rId247" xr:uid="{75763F2A-16D7-DE43-8189-19623CE26370}"/>
+    <hyperlink ref="B281" r:id="rId248" xr:uid="{9263AA30-472A-0A4D-BADF-96D82BB9BFCC}"/>
+    <hyperlink ref="B282" r:id="rId249" xr:uid="{2EF025C3-75C8-564E-BA8B-708C32B0E602}"/>
+    <hyperlink ref="B283" r:id="rId250" xr:uid="{6BDFDCA9-3421-F24F-8EF2-A72742F0AC21}"/>
+    <hyperlink ref="B284" r:id="rId251" xr:uid="{D8447F99-5FF9-D544-99BB-E9969B4A38D7}"/>
+    <hyperlink ref="B285" r:id="rId252" xr:uid="{1DB7EFDA-6C7D-F546-9EE1-F61ED0F65209}"/>
+    <hyperlink ref="B286" r:id="rId253" xr:uid="{D1505609-27D1-784D-ACF6-AE9D0DA2E1B6}"/>
+    <hyperlink ref="B287" r:id="rId254" xr:uid="{6BFA7B45-17D0-4E49-85DA-23C7255A306D}"/>
+    <hyperlink ref="B288" r:id="rId255" xr:uid="{3324BA4A-30CA-5246-8C3C-6505A6987939}"/>
+    <hyperlink ref="B289" r:id="rId256" xr:uid="{894486AD-2B6D-5740-BCAF-0BA1AFF814B4}"/>
+    <hyperlink ref="B290" r:id="rId257" xr:uid="{C47B203B-8B5A-E740-8C86-0784AD28089E}"/>
+    <hyperlink ref="B291" r:id="rId258" xr:uid="{06DC2E54-7597-AE4D-ACDB-B8883A989A4F}"/>
+    <hyperlink ref="B292" r:id="rId259" xr:uid="{E3384259-7CA7-1C44-A66D-11346EE6742E}"/>
+    <hyperlink ref="B293" r:id="rId260" xr:uid="{A5B77769-38AF-3D47-A76B-311591B57D91}"/>
+    <hyperlink ref="B296" r:id="rId261" xr:uid="{9DB6976A-C646-1341-90E8-3A164521267A}"/>
+    <hyperlink ref="B297" r:id="rId262" xr:uid="{03C291F8-D19A-304B-9EF9-CF71A1F66E49}"/>
+    <hyperlink ref="B298" r:id="rId263" xr:uid="{7536415C-140B-9244-B0B2-23F3ED0B2D80}"/>
+    <hyperlink ref="B299" r:id="rId264" xr:uid="{7DBDA456-8AF6-DD43-9764-17D3959B8E8F}"/>
+    <hyperlink ref="B300" r:id="rId265" xr:uid="{BFC149AB-C15A-B648-9F6A-ECD3890B1918}"/>
+    <hyperlink ref="B301" r:id="rId266" xr:uid="{0482240B-FEE9-F746-8980-52BCB7BBB56E}"/>
+    <hyperlink ref="B302" r:id="rId267" xr:uid="{86D1231A-E7C8-4B45-99ED-2DB0EF71E190}"/>
+    <hyperlink ref="B303" r:id="rId268" xr:uid="{20B7CE89-CB37-0040-989F-C8D1BE2B8782}"/>
+    <hyperlink ref="B304" r:id="rId269" xr:uid="{4C8412C9-A47B-9244-A18B-741516BD1054}"/>
+    <hyperlink ref="B305" r:id="rId270" xr:uid="{511761D9-31CE-0B43-AFFD-C011C27ACC52}"/>
+    <hyperlink ref="B306" r:id="rId271" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{6905F997-D048-1049-BA27-C48756603D1E}"/>
+    <hyperlink ref="B307" r:id="rId272" xr:uid="{E657AA82-7CFE-DB42-B20F-F63D8C25EAB6}"/>
+    <hyperlink ref="B308" r:id="rId273" xr:uid="{3E505033-58F3-8F4E-AB82-E12DBC226AEA}"/>
+    <hyperlink ref="B309" r:id="rId274" xr:uid="{749599E5-4972-7343-B13B-87E26F837470}"/>
+    <hyperlink ref="B310" r:id="rId275" xr:uid="{12AA88DC-22AB-5A49-B28C-F04C8E35A215}"/>
+    <hyperlink ref="B311" r:id="rId276" xr:uid="{5751F0A7-7D9D-4148-820B-5B9659DFE34F}"/>
+    <hyperlink ref="B312" r:id="rId277" xr:uid="{4CA2DBEE-B161-B84D-B3A9-B8BC1B598AF2}"/>
+    <hyperlink ref="B313" r:id="rId278" xr:uid="{A9C1E578-6594-954C-8785-8902E605FC7A}"/>
+    <hyperlink ref="B314" r:id="rId279" xr:uid="{3D45E9B8-6671-A747-8C18-51CF8883170A}"/>
+    <hyperlink ref="B315" r:id="rId280" xr:uid="{4F5EF748-8CD4-0F47-90CE-3C93755BF63D}"/>
+    <hyperlink ref="B316" r:id="rId281" xr:uid="{44053C08-5050-C84B-B016-069B1EF9A43D}"/>
+    <hyperlink ref="B317" r:id="rId282" xr:uid="{ABF38928-736B-1A49-8B8A-1DCA5AAECB2B}"/>
+    <hyperlink ref="B318" r:id="rId283" xr:uid="{52651FAF-F3DC-E949-8AF8-998B9724B7D1}"/>
+    <hyperlink ref="B319" r:id="rId284" xr:uid="{91C6CCEF-3FF7-2C42-B5A0-8F4A403ED198}"/>
+    <hyperlink ref="B320" r:id="rId285" xr:uid="{15C8AF08-1A79-F949-9BE7-DD240CBD9861}"/>
+    <hyperlink ref="B321" r:id="rId286" xr:uid="{1904F984-5B22-8D46-BC33-3073B390E8F9}"/>
+    <hyperlink ref="B322" r:id="rId287" xr:uid="{A8BFB3A4-426B-E646-BCF0-FE19C8CD07A9}"/>
+    <hyperlink ref="B323" r:id="rId288" xr:uid="{FBBA29BB-885B-744A-A644-58EDCA7B140A}"/>
+    <hyperlink ref="B324" r:id="rId289" xr:uid="{75411687-6884-AC42-8B4A-1348C4837365}"/>
+    <hyperlink ref="B325" r:id="rId290" xr:uid="{A89ED8DF-F678-FE43-808C-C190721379BF}"/>
+    <hyperlink ref="B326" r:id="rId291" xr:uid="{1516834D-F3B2-1743-8811-263E11BBDEF8}"/>
+    <hyperlink ref="B327" r:id="rId292" xr:uid="{1659AB91-08CA-E44D-988D-E9D9A746D406}"/>
+    <hyperlink ref="B328" r:id="rId293" xr:uid="{E844BC1D-9713-9F4D-B0A4-1124A9952D14}"/>
+    <hyperlink ref="B329" r:id="rId294" xr:uid="{DCE2AAEF-8D8E-1843-BFE9-E9B7E13854EB}"/>
+    <hyperlink ref="B330" r:id="rId295" xr:uid="{836B3BF0-7711-7D41-9E72-914C1871397F}"/>
+    <hyperlink ref="B331" r:id="rId296" xr:uid="{F450CF9B-CA59-1443-8163-13F1121DCF12}"/>
+    <hyperlink ref="B332" r:id="rId297" xr:uid="{1539C3E8-4854-3C4F-A7B3-55BF931F1E2A}"/>
+    <hyperlink ref="B333" r:id="rId298" xr:uid="{04F1FC5F-5DA1-0144-962D-B38C1C41F0F4}"/>
+    <hyperlink ref="B336" r:id="rId299" xr:uid="{B21618F4-70E2-C549-80B7-7CF915679E0A}"/>
+    <hyperlink ref="B337" r:id="rId300" xr:uid="{EEDFBF11-C1E4-0847-9D56-94A72D97AEE7}"/>
+    <hyperlink ref="B338" r:id="rId301" xr:uid="{F5C0EDF1-7EAC-8849-8D27-C3389913BFC6}"/>
+    <hyperlink ref="B339" r:id="rId302" xr:uid="{50175B29-124F-4E4E-8E98-961BD3320359}"/>
+    <hyperlink ref="B340" r:id="rId303" xr:uid="{1BE23822-8512-014F-9154-F6EDA4FC8428}"/>
+    <hyperlink ref="B341" r:id="rId304" xr:uid="{38EC228E-ABFF-3542-9CFB-3DDFC628E9D0}"/>
+    <hyperlink ref="B342" r:id="rId305" xr:uid="{73F240F8-C469-454E-BA5C-CFF2F7A7A5F6}"/>
+    <hyperlink ref="B343" r:id="rId306" xr:uid="{3BBD1BAC-68C7-A94A-9063-AF62B5C837FD}"/>
+    <hyperlink ref="B344" r:id="rId307" xr:uid="{F9751D9B-2689-E24B-9FC3-CA32FE888708}"/>
+    <hyperlink ref="B345" r:id="rId308" xr:uid="{73C61D6A-D97C-B944-8B27-BB91564AB0D7}"/>
+    <hyperlink ref="B346" r:id="rId309" xr:uid="{936E077C-C016-A04F-895A-782D6D9D9433}"/>
+    <hyperlink ref="B347" r:id="rId310" xr:uid="{5454A2A1-6607-BE48-9215-CB8965EC3568}"/>
+    <hyperlink ref="B348" r:id="rId311" xr:uid="{FC1EAA10-F7ED-6B42-A79B-3D8B44E2C8B3}"/>
+    <hyperlink ref="B349" r:id="rId312" xr:uid="{FDB7F712-4A42-1048-8929-A1E752B07C6A}"/>
+    <hyperlink ref="B350" r:id="rId313" xr:uid="{AF3ACA60-0B0E-E146-B51F-A2CD05EB6549}"/>
+    <hyperlink ref="B351" r:id="rId314" xr:uid="{BB63E040-7A1A-E046-9BDD-9CBD1DA89DE9}"/>
+    <hyperlink ref="B352" r:id="rId315" xr:uid="{9AF8FD93-CCC9-D540-AE9A-00583F309649}"/>
+    <hyperlink ref="B353" r:id="rId316" xr:uid="{66A746A0-71FE-E546-92B7-D1C3D582E067}"/>
+    <hyperlink ref="B357" r:id="rId317" xr:uid="{BD79CCE1-5315-3944-9F9B-618615EC4583}"/>
+    <hyperlink ref="B358" r:id="rId318" xr:uid="{A5068A51-C961-6847-BB27-40A850B6D393}"/>
+    <hyperlink ref="B359" r:id="rId319" xr:uid="{6B8D36F0-E796-B944-A456-E8A9E2EE0BDB}"/>
+    <hyperlink ref="B360" r:id="rId320" xr:uid="{776652B7-2C11-4641-BF6A-EABEEB9B55AB}"/>
+    <hyperlink ref="B361" r:id="rId321" xr:uid="{95C6B35D-712A-2343-B790-236B55C5EC49}"/>
+    <hyperlink ref="B362" r:id="rId322" xr:uid="{4ED53872-1FE9-F140-AA35-F228F762880B}"/>
+    <hyperlink ref="B363" r:id="rId323" xr:uid="{6D5E6A28-85AA-BF4C-B2BD-9378D6E28EC7}"/>
+    <hyperlink ref="B364" r:id="rId324" xr:uid="{BCAD1ECB-15EE-CF49-878E-AA682DE3AC22}"/>
+    <hyperlink ref="B365" r:id="rId325" xr:uid="{C85468B5-25E9-E446-808E-72CFE911F0C2}"/>
+    <hyperlink ref="B366" r:id="rId326" xr:uid="{9503AECA-1A6A-9640-A04C-4CEAA2304448}"/>
+    <hyperlink ref="B367" r:id="rId327" xr:uid="{74211516-06B0-AA45-845B-52C8202751DA}"/>
+    <hyperlink ref="B368" r:id="rId328" xr:uid="{02C696BC-4B91-9444-900F-9CD68E409ABC}"/>
+    <hyperlink ref="B369" r:id="rId329" xr:uid="{04646C45-4118-374C-839D-94D31D534FAC}"/>
+    <hyperlink ref="B370" r:id="rId330" xr:uid="{F90BCCAE-8596-FC4D-BDD7-774392C596DF}"/>
+    <hyperlink ref="B371" r:id="rId331" xr:uid="{65230925-36EC-8A4B-8E46-6350B9BC0F95}"/>
+    <hyperlink ref="B372" r:id="rId332" xr:uid="{E91B8177-0C7A-1F40-BD34-4CC60F03B84F}"/>
+    <hyperlink ref="B373" r:id="rId333" xr:uid="{E8CBFD60-7335-0B4D-9FF5-99B4A8DC551D}"/>
+    <hyperlink ref="B374" r:id="rId334" xr:uid="{A35F55D4-9B87-C745-94DB-E7D820193C30}"/>
+    <hyperlink ref="B375" r:id="rId335" xr:uid="{6461A29F-D404-334F-B13F-296B4CA5E8A4}"/>
+    <hyperlink ref="B376" r:id="rId336" xr:uid="{FA9B4BE7-85CC-B24F-9461-5E9B42DDD824}"/>
+    <hyperlink ref="B377" r:id="rId337" xr:uid="{A75ACEA2-CDF6-A147-8540-A6DF55B15F45}"/>
+    <hyperlink ref="B378" r:id="rId338" xr:uid="{62FF87E2-E658-AB4D-AC57-7BCF9D49516E}"/>
+    <hyperlink ref="B379" r:id="rId339" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
+    <hyperlink ref="B380" r:id="rId340" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
+    <hyperlink ref="B381" r:id="rId341" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
+    <hyperlink ref="B382" r:id="rId342" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
+    <hyperlink ref="B383" r:id="rId343" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
+    <hyperlink ref="B384" r:id="rId344" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
+    <hyperlink ref="B385" r:id="rId345" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
+    <hyperlink ref="B386" r:id="rId346" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
+    <hyperlink ref="B387" r:id="rId347" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
+    <hyperlink ref="B388" r:id="rId348" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
+    <hyperlink ref="B389" r:id="rId349" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
+    <hyperlink ref="B390" r:id="rId350" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
+    <hyperlink ref="B391" r:id="rId351" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
+    <hyperlink ref="B392" r:id="rId352" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
+    <hyperlink ref="B393" r:id="rId353" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
+    <hyperlink ref="B394" r:id="rId354" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
+    <hyperlink ref="B396" r:id="rId355" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
+    <hyperlink ref="B395" r:id="rId356" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
+    <hyperlink ref="B397" r:id="rId357" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
+    <hyperlink ref="B398" r:id="rId358" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
+    <hyperlink ref="B399" r:id="rId359" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
+    <hyperlink ref="B402" r:id="rId360" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
+    <hyperlink ref="B403" r:id="rId361" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
+    <hyperlink ref="B404" r:id="rId362" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
+    <hyperlink ref="B405" r:id="rId363" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
+    <hyperlink ref="B406" r:id="rId364" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
+    <hyperlink ref="B407" r:id="rId365" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
+    <hyperlink ref="B410" r:id="rId366" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
+    <hyperlink ref="B411" r:id="rId367" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
+    <hyperlink ref="B412" r:id="rId368" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
+    <hyperlink ref="B413" r:id="rId369" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
+    <hyperlink ref="B414" r:id="rId370" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
+    <hyperlink ref="B415" r:id="rId371" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
+    <hyperlink ref="B416" r:id="rId372" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
+    <hyperlink ref="B417" r:id="rId373" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
+    <hyperlink ref="B418" r:id="rId374" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
+    <hyperlink ref="B419" r:id="rId375" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
+    <hyperlink ref="B420" r:id="rId376" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
+    <hyperlink ref="B421" r:id="rId377" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
+    <hyperlink ref="B422" r:id="rId378" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
+    <hyperlink ref="B423" r:id="rId379" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
+    <hyperlink ref="B424" r:id="rId380" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
+    <hyperlink ref="B425" r:id="rId381" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
+    <hyperlink ref="B426" r:id="rId382" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
+    <hyperlink ref="B427" r:id="rId383" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
+    <hyperlink ref="B428" r:id="rId384" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
+    <hyperlink ref="B429" r:id="rId385" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
+    <hyperlink ref="B430" r:id="rId386" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
+    <hyperlink ref="B431" r:id="rId387" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
+    <hyperlink ref="B432" r:id="rId388" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
+    <hyperlink ref="B433" r:id="rId389" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
+    <hyperlink ref="B434" r:id="rId390" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
+    <hyperlink ref="B435" r:id="rId391" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
+    <hyperlink ref="B436" r:id="rId392" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
+    <hyperlink ref="B437" r:id="rId393" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
+    <hyperlink ref="B438" r:id="rId394" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
+    <hyperlink ref="B439" r:id="rId395" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
+    <hyperlink ref="B440" r:id="rId396" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
+    <hyperlink ref="B441" r:id="rId397" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
+    <hyperlink ref="B442" r:id="rId398" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
+    <hyperlink ref="B443" r:id="rId399" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
+    <hyperlink ref="B444" r:id="rId400" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
+    <hyperlink ref="B445" r:id="rId401" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
+    <hyperlink ref="B446" r:id="rId402" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
+    <hyperlink ref="B447" r:id="rId403" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
+    <hyperlink ref="B448" r:id="rId404" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
+    <hyperlink ref="B449" r:id="rId405" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
+    <hyperlink ref="B451" r:id="rId406" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
+    <hyperlink ref="B450" r:id="rId407" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
+    <hyperlink ref="B452" r:id="rId408" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
+    <hyperlink ref="B453" r:id="rId409" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
+    <hyperlink ref="B454" r:id="rId410" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
+    <hyperlink ref="B455" r:id="rId411" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
+    <hyperlink ref="B456" r:id="rId412" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
+    <hyperlink ref="B457" r:id="rId413" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
+    <hyperlink ref="B458" r:id="rId414" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
+    <hyperlink ref="B459" r:id="rId415" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
+    <hyperlink ref="B460" r:id="rId416" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
+    <hyperlink ref="B461" r:id="rId417" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
+    <hyperlink ref="B462" r:id="rId418" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
+    <hyperlink ref="B469" r:id="rId419" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
+    <hyperlink ref="B468" r:id="rId420" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
+    <hyperlink ref="B467" r:id="rId421" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
+    <hyperlink ref="B466" r:id="rId422" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
+    <hyperlink ref="B465" r:id="rId423" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
+    <hyperlink ref="B464" r:id="rId424" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
+    <hyperlink ref="B463" r:id="rId425" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
+    <hyperlink ref="B472" r:id="rId426" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
+    <hyperlink ref="B473" r:id="rId427" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
+    <hyperlink ref="B474" r:id="rId428" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
+    <hyperlink ref="B475" r:id="rId429" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
+    <hyperlink ref="B476" r:id="rId430" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
+    <hyperlink ref="B477" r:id="rId431" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
+    <hyperlink ref="B478" r:id="rId432" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
+    <hyperlink ref="B481" r:id="rId433" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
+    <hyperlink ref="B479" r:id="rId434" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
+    <hyperlink ref="B480" r:id="rId435" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
+    <hyperlink ref="B356" r:id="rId436" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
+    <hyperlink ref="B2" r:id="rId437" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
+    <hyperlink ref="B95" r:id="rId438" xr:uid="{1F507CBC-4056-AD46-9314-95ECBB9D799D}"/>
+    <hyperlink ref="B94" r:id="rId439" xr:uid="{AB28D9E6-890C-F14A-A5FB-2303BE319968}"/>
+    <hyperlink ref="B93" r:id="rId440" xr:uid="{B9AC5194-6D36-684A-A5C4-BEE11037599F}"/>
+    <hyperlink ref="B92" r:id="rId441" xr:uid="{C8C607BB-1FEE-FA47-9E3E-6C0BCE978B7F}"/>
+    <hyperlink ref="B91" r:id="rId442" xr:uid="{2D956AC4-4774-7446-8473-C4CE00E33C17}"/>
+    <hyperlink ref="B90" r:id="rId443" xr:uid="{ED0F5FC7-0066-EB44-8FCF-460600DADB02}"/>
+    <hyperlink ref="B89" r:id="rId444" xr:uid="{A3D51762-65A1-9A44-B619-D1D98A7F403B}"/>
+    <hyperlink ref="B88" r:id="rId445" xr:uid="{8E3D4BDF-9F8F-0542-BFD8-C3CE3BF396E6}"/>
+    <hyperlink ref="B87" r:id="rId446" xr:uid="{62982242-1D19-1544-8653-8E25E9BF4505}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId447"/>

</xml_diff>

<commit_message>
37, 38 and 39
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCF6302-C8C2-43FE-8BC9-4AFD64FC528A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AB1E17-CD4A-4F57-8A91-FB75D808802E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1923,8 +1923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2870,8 +2870,8 @@
       <c r="B91" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C91" s="4" t="s">
-        <v>4</v>
+      <c r="C91" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="21">
@@ -2881,8 +2881,8 @@
       <c r="B92" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C92" s="4" t="s">
-        <v>4</v>
+      <c r="C92" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="21">
@@ -2892,8 +2892,8 @@
       <c r="B93" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C93" s="4" t="s">
-        <v>4</v>
+      <c r="C93" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="21">
@@ -2903,8 +2903,8 @@
       <c r="B94" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C94" s="4" t="s">
-        <v>4</v>
+      <c r="C94" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 40, 41 and 42
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AB1E17-CD4A-4F57-8A91-FB75D808802E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F679B1-3CE7-4FBA-9BA8-6976168A6877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1435,7 +1435,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1493,6 +1493,12 @@
       <b/>
       <sz val="15"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1561,7 +1567,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1604,6 +1610,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1923,8 +1932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" topLeftCell="A476" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B499" sqref="B499"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2914,8 +2923,8 @@
       <c r="B95" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C95" s="4" t="s">
-        <v>4</v>
+      <c r="C95" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="21">
@@ -2925,8 +2934,8 @@
       <c r="B96" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C96" s="4" t="s">
-        <v>4</v>
+      <c r="C96" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="21">
@@ -2936,8 +2945,8 @@
       <c r="B97" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C97" s="4" t="s">
-        <v>4</v>
+      <c r="C97" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="21">
@@ -2947,8 +2956,8 @@
       <c r="B98" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C98" s="4" t="s">
-        <v>4</v>
+      <c r="C98" s="18" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 43 and 44
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F679B1-3CE7-4FBA-9BA8-6976168A6877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB27648C-D3D2-4A75-8146-D8951FB8DA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="467">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1429,6 +1429,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
 </sst>
 </file>
@@ -1932,8 +1935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A476" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B499" sqref="B499"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2972,8 +2975,8 @@
       <c r="B101" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C101" s="4" t="s">
-        <v>4</v>
+      <c r="C101" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="21">
@@ -2983,8 +2986,8 @@
       <c r="B102" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C102" s="4" t="s">
-        <v>4</v>
+      <c r="C102" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="21">
@@ -2994,8 +2997,8 @@
       <c r="B103" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C103" s="4" t="s">
-        <v>4</v>
+      <c r="C103" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="21">
@@ -3005,8 +3008,8 @@
       <c r="B104" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C104" s="4" t="s">
-        <v>4</v>
+      <c r="C104" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="21">
@@ -3028,7 +3031,7 @@
         <v>103</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 53 and 54
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0572288C-C411-4F1E-9FFE-23C532DAD456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F67BDCE-29BC-4584-8869-A1CCC242EF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1944,8 +1944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C136" sqref="C136"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3384,8 +3384,8 @@
       <c r="B139" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C139" s="4" t="s">
-        <v>4</v>
+      <c r="C139" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="21">
@@ -3395,8 +3395,8 @@
       <c r="B140" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C140" s="4" t="s">
-        <v>4</v>
+      <c r="C140" s="13" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="21">
@@ -3406,8 +3406,8 @@
       <c r="B141" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="C141" s="4" t="s">
-        <v>4</v>
+      <c r="C141" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="21">
@@ -3417,8 +3417,8 @@
       <c r="B142" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="C142" s="4" t="s">
-        <v>4</v>
+      <c r="C142" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 66, 67 and 68
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3833D65-5F32-4D2A-9883-0B1D4B493B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F288CC93-C8DA-4E79-8B41-6AE07800BBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1959,8 +1959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C244" sqref="C244"/>
+    <sheetView tabSelected="1" topLeftCell="A249" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B258" sqref="B258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -4598,8 +4598,8 @@
       <c r="B252" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="C252" s="4" t="s">
-        <v>4</v>
+      <c r="C252" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="253" spans="1:3" ht="21">
@@ -4609,8 +4609,8 @@
       <c r="B253" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="C253" s="4" t="s">
-        <v>4</v>
+      <c r="C253" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="254" spans="1:3" ht="21">
@@ -4620,8 +4620,8 @@
       <c r="B254" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="C254" s="4" t="s">
-        <v>4</v>
+      <c r="C254" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="255" spans="1:3" ht="21">
@@ -4631,8 +4631,8 @@
       <c r="B255" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="C255" s="4" t="s">
-        <v>4</v>
+      <c r="C255" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="256" spans="1:3" ht="21">
@@ -4642,8 +4642,8 @@
       <c r="B256" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="C256" s="4" t="s">
-        <v>4</v>
+      <c r="C256" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="257" spans="1:3" ht="21">
@@ -4653,8 +4653,8 @@
       <c r="B257" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="C257" s="4" t="s">
-        <v>4</v>
+      <c r="C257" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="258" spans="1:3" ht="21">
@@ -4664,8 +4664,8 @@
       <c r="B258" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="C258" s="4" t="s">
-        <v>4</v>
+      <c r="C258" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="259" spans="1:3" ht="21">
@@ -4675,8 +4675,8 @@
       <c r="B259" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="C259" s="4" t="s">
-        <v>4</v>
+      <c r="C259" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="260" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 70 and 71
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D03E5A-4E93-4080-B04B-9757A8225523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC97F152-240B-4F8E-ABEE-B86F103B3AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1959,8 +1959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A249" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C260" sqref="C260"/>
+    <sheetView tabSelected="1" topLeftCell="A259" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B272" sqref="B272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -4730,8 +4730,8 @@
       <c r="B264" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="C264" s="4" t="s">
-        <v>4</v>
+      <c r="C264" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="265" spans="1:3" ht="21">
@@ -4741,8 +4741,8 @@
       <c r="B265" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="C265" s="4" t="s">
-        <v>4</v>
+      <c r="C265" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="266" spans="1:3" ht="21">
@@ -4752,8 +4752,8 @@
       <c r="B266" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="C266" s="4" t="s">
-        <v>4</v>
+      <c r="C266" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="267" spans="1:3" ht="21">
@@ -4763,8 +4763,8 @@
       <c r="B267" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="C267" s="4" t="s">
-        <v>4</v>
+      <c r="C267" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="268" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 73 and 74
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130884C5-9DBD-437B-B0F7-7FB95B00ECF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4FA43F-0A78-46E9-928C-78502205600F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1972,7 +1972,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A268" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B261" sqref="B261"/>
+      <selection activeCell="C281" sqref="C281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -4849,8 +4849,8 @@
       <c r="B275" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="C275" s="4" t="s">
-        <v>4</v>
+      <c r="C275" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="276" spans="1:3" ht="21">
@@ -4860,8 +4860,8 @@
       <c r="B276" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="C276" s="4" t="s">
-        <v>4</v>
+      <c r="C276" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="277" spans="1:3" ht="21">
@@ -4871,8 +4871,8 @@
       <c r="B277" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="C277" s="4" t="s">
-        <v>4</v>
+      <c r="C277" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="278" spans="1:3" ht="21">
@@ -4882,8 +4882,8 @@
       <c r="B278" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="C278" s="4" t="s">
-        <v>4</v>
+      <c r="C278" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="279" spans="1:3" ht="21">
@@ -4893,8 +4893,8 @@
       <c r="B279" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="C279" s="4" t="s">
-        <v>4</v>
+      <c r="C279" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="280" spans="1:3" ht="21">
@@ -4904,8 +4904,8 @@
       <c r="B280" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="C280" s="4" t="s">
-        <v>4</v>
+      <c r="C280" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="281" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 82 and 83
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39E3CF2-3391-42CA-99CE-88A834248032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE21F388-9548-476C-AF98-FB8E557AF068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1971,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A282" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C292" sqref="C292"/>
+    <sheetView tabSelected="1" topLeftCell="A357" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C365" sqref="C365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5698,8 +5698,8 @@
       <c r="B356" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="C356" s="4" t="s">
-        <v>4</v>
+      <c r="C356" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="357" spans="1:3" ht="21">
@@ -5709,8 +5709,8 @@
       <c r="B357" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="C357" s="4" t="s">
-        <v>4</v>
+      <c r="C357" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="358" spans="1:3" ht="21">
@@ -5720,8 +5720,8 @@
       <c r="B358" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="C358" s="4" t="s">
-        <v>4</v>
+      <c r="C358" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="359" spans="1:3" ht="21">
@@ -5731,8 +5731,8 @@
       <c r="B359" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="C359" s="4" t="s">
-        <v>4</v>
+      <c r="C359" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="360" spans="1:3" ht="21">
@@ -5742,8 +5742,8 @@
       <c r="B360" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="C360" s="4" t="s">
-        <v>4</v>
+      <c r="C360" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="361" spans="1:3" ht="21">
@@ -5753,8 +5753,8 @@
       <c r="B361" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="C361" s="4" t="s">
-        <v>4</v>
+      <c r="C361" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="362" spans="1:3" ht="21">
@@ -5764,8 +5764,8 @@
       <c r="B362" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="C362" s="4" t="s">
-        <v>4</v>
+      <c r="C362" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="363" spans="1:3" ht="21">
@@ -5775,8 +5775,8 @@
       <c r="B363" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="C363" s="4" t="s">
-        <v>4</v>
+      <c r="C363" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="364" spans="1:3" ht="21">
@@ -5786,8 +5786,8 @@
       <c r="B364" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="C364" s="4" t="s">
-        <v>4</v>
+      <c r="C364" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="365" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 85, 86 and 87
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3A379E-9BE8-4196-A234-8953C785C925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783B09A5-9924-4DAE-8CE5-BEEB8F60B43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1971,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A362" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C370" sqref="C370"/>
+    <sheetView tabSelected="1" topLeftCell="A369" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C380" sqref="C380"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5885,8 +5885,8 @@
       <c r="B373" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="C373" s="4" t="s">
-        <v>4</v>
+      <c r="C373" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="374" spans="1:3" ht="21">
@@ -5896,8 +5896,8 @@
       <c r="B374" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="C374" s="4" t="s">
-        <v>4</v>
+      <c r="C374" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="375" spans="1:3" ht="21">
@@ -5907,8 +5907,8 @@
       <c r="B375" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="C375" s="4" t="s">
-        <v>4</v>
+      <c r="C375" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="376" spans="1:3" ht="21">
@@ -5918,8 +5918,8 @@
       <c r="B376" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="C376" s="4" t="s">
-        <v>4</v>
+      <c r="C376" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="377" spans="1:3" ht="21">
@@ -5929,8 +5929,8 @@
       <c r="B377" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="C377" s="4" t="s">
-        <v>4</v>
+      <c r="C377" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="378" spans="1:3" ht="21">
@@ -5940,8 +5940,8 @@
       <c r="B378" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="C378" s="4" t="s">
-        <v>4</v>
+      <c r="C378" s="13" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="379" spans="1:3" ht="21">
@@ -5951,8 +5951,8 @@
       <c r="B379" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="C379" s="4" t="s">
-        <v>4</v>
+      <c r="C379" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="380" spans="1:3" ht="21">
@@ -5962,8 +5962,8 @@
       <c r="B380" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="C380" s="4" t="s">
-        <v>4</v>
+      <c r="C380" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="381" spans="1:3" ht="21">
@@ -5973,8 +5973,8 @@
       <c r="B381" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="C381" s="4" t="s">
-        <v>4</v>
+      <c r="C381" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="382" spans="1:3" ht="21">
@@ -7370,120 +7370,120 @@
     <hyperlink ref="B371" r:id="rId330" xr:uid="{65230925-36EC-8A4B-8E46-6350B9BC0F95}"/>
     <hyperlink ref="B372" r:id="rId331" xr:uid="{E91B8177-0C7A-1F40-BD34-4CC60F03B84F}"/>
     <hyperlink ref="B373" r:id="rId332" xr:uid="{E8CBFD60-7335-0B4D-9FF5-99B4A8DC551D}"/>
-    <hyperlink ref="B374" r:id="rId333" xr:uid="{A35F55D4-9B87-C745-94DB-E7D820193C30}"/>
-    <hyperlink ref="B375" r:id="rId334" xr:uid="{6461A29F-D404-334F-B13F-296B4CA5E8A4}"/>
-    <hyperlink ref="B376" r:id="rId335" xr:uid="{FA9B4BE7-85CC-B24F-9461-5E9B42DDD824}"/>
-    <hyperlink ref="B377" r:id="rId336" xr:uid="{A75ACEA2-CDF6-A147-8540-A6DF55B15F45}"/>
-    <hyperlink ref="B378" r:id="rId337" xr:uid="{62FF87E2-E658-AB4D-AC57-7BCF9D49516E}"/>
-    <hyperlink ref="B379" r:id="rId338" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
-    <hyperlink ref="B380" r:id="rId339" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
-    <hyperlink ref="B381" r:id="rId340" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
-    <hyperlink ref="B382" r:id="rId341" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
-    <hyperlink ref="B383" r:id="rId342" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
-    <hyperlink ref="B384" r:id="rId343" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
-    <hyperlink ref="B385" r:id="rId344" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
-    <hyperlink ref="B386" r:id="rId345" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
-    <hyperlink ref="B387" r:id="rId346" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
-    <hyperlink ref="B388" r:id="rId347" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
-    <hyperlink ref="B389" r:id="rId348" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
-    <hyperlink ref="B390" r:id="rId349" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
-    <hyperlink ref="B391" r:id="rId350" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
-    <hyperlink ref="B392" r:id="rId351" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
-    <hyperlink ref="B393" r:id="rId352" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
-    <hyperlink ref="B394" r:id="rId353" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
-    <hyperlink ref="B396" r:id="rId354" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
-    <hyperlink ref="B395" r:id="rId355" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
-    <hyperlink ref="B397" r:id="rId356" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
-    <hyperlink ref="B398" r:id="rId357" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
-    <hyperlink ref="B399" r:id="rId358" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
-    <hyperlink ref="B402" r:id="rId359" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
-    <hyperlink ref="B403" r:id="rId360" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
-    <hyperlink ref="B404" r:id="rId361" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
-    <hyperlink ref="B405" r:id="rId362" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
-    <hyperlink ref="B406" r:id="rId363" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
-    <hyperlink ref="B407" r:id="rId364" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
-    <hyperlink ref="B410" r:id="rId365" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
-    <hyperlink ref="B411" r:id="rId366" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
-    <hyperlink ref="B412" r:id="rId367" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
-    <hyperlink ref="B413" r:id="rId368" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
-    <hyperlink ref="B414" r:id="rId369" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
-    <hyperlink ref="B415" r:id="rId370" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
-    <hyperlink ref="B416" r:id="rId371" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
-    <hyperlink ref="B417" r:id="rId372" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
-    <hyperlink ref="B418" r:id="rId373" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
-    <hyperlink ref="B419" r:id="rId374" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
-    <hyperlink ref="B420" r:id="rId375" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
-    <hyperlink ref="B421" r:id="rId376" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
-    <hyperlink ref="B422" r:id="rId377" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
-    <hyperlink ref="B423" r:id="rId378" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
-    <hyperlink ref="B424" r:id="rId379" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
-    <hyperlink ref="B425" r:id="rId380" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
-    <hyperlink ref="B426" r:id="rId381" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
-    <hyperlink ref="B427" r:id="rId382" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
-    <hyperlink ref="B428" r:id="rId383" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
-    <hyperlink ref="B429" r:id="rId384" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
-    <hyperlink ref="B430" r:id="rId385" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
-    <hyperlink ref="B431" r:id="rId386" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
-    <hyperlink ref="B432" r:id="rId387" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
-    <hyperlink ref="B433" r:id="rId388" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
-    <hyperlink ref="B434" r:id="rId389" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
-    <hyperlink ref="B435" r:id="rId390" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
-    <hyperlink ref="B436" r:id="rId391" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
-    <hyperlink ref="B437" r:id="rId392" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
-    <hyperlink ref="B438" r:id="rId393" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
-    <hyperlink ref="B439" r:id="rId394" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
-    <hyperlink ref="B440" r:id="rId395" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
-    <hyperlink ref="B441" r:id="rId396" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
-    <hyperlink ref="B442" r:id="rId397" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
-    <hyperlink ref="B443" r:id="rId398" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
-    <hyperlink ref="B444" r:id="rId399" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
-    <hyperlink ref="B445" r:id="rId400" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
-    <hyperlink ref="B446" r:id="rId401" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
-    <hyperlink ref="B447" r:id="rId402" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
-    <hyperlink ref="B448" r:id="rId403" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
-    <hyperlink ref="B449" r:id="rId404" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
-    <hyperlink ref="B451" r:id="rId405" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
-    <hyperlink ref="B450" r:id="rId406" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
-    <hyperlink ref="B452" r:id="rId407" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
-    <hyperlink ref="B453" r:id="rId408" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
-    <hyperlink ref="B454" r:id="rId409" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
-    <hyperlink ref="B455" r:id="rId410" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
-    <hyperlink ref="B456" r:id="rId411" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
-    <hyperlink ref="B457" r:id="rId412" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
-    <hyperlink ref="B458" r:id="rId413" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
-    <hyperlink ref="B459" r:id="rId414" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
-    <hyperlink ref="B460" r:id="rId415" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
-    <hyperlink ref="B461" r:id="rId416" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
-    <hyperlink ref="B462" r:id="rId417" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
-    <hyperlink ref="B469" r:id="rId418" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
-    <hyperlink ref="B468" r:id="rId419" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
-    <hyperlink ref="B467" r:id="rId420" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
-    <hyperlink ref="B466" r:id="rId421" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
-    <hyperlink ref="B465" r:id="rId422" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
-    <hyperlink ref="B464" r:id="rId423" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
-    <hyperlink ref="B463" r:id="rId424" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
-    <hyperlink ref="B472" r:id="rId425" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
-    <hyperlink ref="B473" r:id="rId426" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
-    <hyperlink ref="B474" r:id="rId427" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
-    <hyperlink ref="B475" r:id="rId428" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
-    <hyperlink ref="B476" r:id="rId429" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
-    <hyperlink ref="B477" r:id="rId430" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
-    <hyperlink ref="B478" r:id="rId431" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="B481" r:id="rId432" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
-    <hyperlink ref="B479" r:id="rId433" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
-    <hyperlink ref="B480" r:id="rId434" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
-    <hyperlink ref="B356" r:id="rId435" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
-    <hyperlink ref="B2" r:id="rId436" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
-    <hyperlink ref="B95" r:id="rId437" xr:uid="{1F507CBC-4056-AD46-9314-95ECBB9D799D}"/>
-    <hyperlink ref="B94" r:id="rId438" xr:uid="{AB28D9E6-890C-F14A-A5FB-2303BE319968}"/>
-    <hyperlink ref="B93" r:id="rId439" xr:uid="{B9AC5194-6D36-684A-A5C4-BEE11037599F}"/>
-    <hyperlink ref="B92" r:id="rId440" xr:uid="{C8C607BB-1FEE-FA47-9E3E-6C0BCE978B7F}"/>
-    <hyperlink ref="B91" r:id="rId441" xr:uid="{2D956AC4-4774-7446-8473-C4CE00E33C17}"/>
-    <hyperlink ref="B90" r:id="rId442" xr:uid="{ED0F5FC7-0066-EB44-8FCF-460600DADB02}"/>
-    <hyperlink ref="B89" r:id="rId443" xr:uid="{A3D51762-65A1-9A44-B619-D1D98A7F403B}"/>
-    <hyperlink ref="B88" r:id="rId444" xr:uid="{8E3D4BDF-9F8F-0542-BFD8-C3CE3BF396E6}"/>
-    <hyperlink ref="B87" r:id="rId445" xr:uid="{62982242-1D19-1544-8653-8E25E9BF4505}"/>
-    <hyperlink ref="B292" r:id="rId446" xr:uid="{E3384259-7CA7-1C44-A66D-11346EE6742E}"/>
+    <hyperlink ref="B375" r:id="rId333" xr:uid="{6461A29F-D404-334F-B13F-296B4CA5E8A4}"/>
+    <hyperlink ref="B376" r:id="rId334" xr:uid="{FA9B4BE7-85CC-B24F-9461-5E9B42DDD824}"/>
+    <hyperlink ref="B377" r:id="rId335" xr:uid="{A75ACEA2-CDF6-A147-8540-A6DF55B15F45}"/>
+    <hyperlink ref="B378" r:id="rId336" xr:uid="{62FF87E2-E658-AB4D-AC57-7BCF9D49516E}"/>
+    <hyperlink ref="B379" r:id="rId337" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
+    <hyperlink ref="B380" r:id="rId338" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
+    <hyperlink ref="B381" r:id="rId339" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
+    <hyperlink ref="B382" r:id="rId340" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
+    <hyperlink ref="B383" r:id="rId341" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
+    <hyperlink ref="B384" r:id="rId342" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
+    <hyperlink ref="B385" r:id="rId343" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
+    <hyperlink ref="B386" r:id="rId344" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
+    <hyperlink ref="B387" r:id="rId345" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
+    <hyperlink ref="B388" r:id="rId346" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
+    <hyperlink ref="B389" r:id="rId347" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
+    <hyperlink ref="B390" r:id="rId348" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
+    <hyperlink ref="B391" r:id="rId349" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
+    <hyperlink ref="B392" r:id="rId350" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
+    <hyperlink ref="B393" r:id="rId351" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
+    <hyperlink ref="B394" r:id="rId352" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
+    <hyperlink ref="B396" r:id="rId353" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
+    <hyperlink ref="B395" r:id="rId354" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
+    <hyperlink ref="B397" r:id="rId355" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
+    <hyperlink ref="B398" r:id="rId356" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
+    <hyperlink ref="B399" r:id="rId357" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
+    <hyperlink ref="B402" r:id="rId358" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
+    <hyperlink ref="B403" r:id="rId359" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
+    <hyperlink ref="B404" r:id="rId360" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
+    <hyperlink ref="B405" r:id="rId361" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
+    <hyperlink ref="B406" r:id="rId362" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
+    <hyperlink ref="B407" r:id="rId363" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
+    <hyperlink ref="B410" r:id="rId364" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
+    <hyperlink ref="B411" r:id="rId365" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
+    <hyperlink ref="B412" r:id="rId366" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
+    <hyperlink ref="B413" r:id="rId367" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
+    <hyperlink ref="B414" r:id="rId368" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
+    <hyperlink ref="B415" r:id="rId369" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
+    <hyperlink ref="B416" r:id="rId370" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
+    <hyperlink ref="B417" r:id="rId371" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
+    <hyperlink ref="B418" r:id="rId372" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
+    <hyperlink ref="B419" r:id="rId373" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
+    <hyperlink ref="B420" r:id="rId374" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
+    <hyperlink ref="B421" r:id="rId375" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
+    <hyperlink ref="B422" r:id="rId376" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
+    <hyperlink ref="B423" r:id="rId377" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
+    <hyperlink ref="B424" r:id="rId378" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
+    <hyperlink ref="B425" r:id="rId379" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
+    <hyperlink ref="B426" r:id="rId380" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
+    <hyperlink ref="B427" r:id="rId381" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
+    <hyperlink ref="B428" r:id="rId382" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
+    <hyperlink ref="B429" r:id="rId383" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
+    <hyperlink ref="B430" r:id="rId384" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
+    <hyperlink ref="B431" r:id="rId385" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
+    <hyperlink ref="B432" r:id="rId386" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
+    <hyperlink ref="B433" r:id="rId387" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
+    <hyperlink ref="B434" r:id="rId388" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
+    <hyperlink ref="B435" r:id="rId389" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
+    <hyperlink ref="B436" r:id="rId390" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
+    <hyperlink ref="B437" r:id="rId391" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
+    <hyperlink ref="B438" r:id="rId392" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
+    <hyperlink ref="B439" r:id="rId393" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
+    <hyperlink ref="B440" r:id="rId394" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
+    <hyperlink ref="B441" r:id="rId395" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
+    <hyperlink ref="B442" r:id="rId396" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
+    <hyperlink ref="B443" r:id="rId397" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
+    <hyperlink ref="B444" r:id="rId398" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
+    <hyperlink ref="B445" r:id="rId399" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
+    <hyperlink ref="B446" r:id="rId400" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
+    <hyperlink ref="B447" r:id="rId401" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
+    <hyperlink ref="B448" r:id="rId402" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
+    <hyperlink ref="B449" r:id="rId403" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
+    <hyperlink ref="B451" r:id="rId404" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
+    <hyperlink ref="B450" r:id="rId405" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
+    <hyperlink ref="B452" r:id="rId406" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
+    <hyperlink ref="B453" r:id="rId407" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
+    <hyperlink ref="B454" r:id="rId408" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
+    <hyperlink ref="B455" r:id="rId409" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
+    <hyperlink ref="B456" r:id="rId410" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
+    <hyperlink ref="B457" r:id="rId411" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
+    <hyperlink ref="B458" r:id="rId412" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
+    <hyperlink ref="B459" r:id="rId413" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
+    <hyperlink ref="B460" r:id="rId414" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
+    <hyperlink ref="B461" r:id="rId415" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
+    <hyperlink ref="B462" r:id="rId416" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
+    <hyperlink ref="B469" r:id="rId417" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
+    <hyperlink ref="B468" r:id="rId418" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
+    <hyperlink ref="B467" r:id="rId419" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
+    <hyperlink ref="B466" r:id="rId420" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
+    <hyperlink ref="B465" r:id="rId421" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
+    <hyperlink ref="B464" r:id="rId422" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
+    <hyperlink ref="B463" r:id="rId423" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
+    <hyperlink ref="B472" r:id="rId424" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
+    <hyperlink ref="B473" r:id="rId425" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
+    <hyperlink ref="B474" r:id="rId426" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
+    <hyperlink ref="B475" r:id="rId427" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
+    <hyperlink ref="B476" r:id="rId428" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
+    <hyperlink ref="B477" r:id="rId429" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
+    <hyperlink ref="B478" r:id="rId430" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
+    <hyperlink ref="B481" r:id="rId431" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
+    <hyperlink ref="B479" r:id="rId432" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
+    <hyperlink ref="B480" r:id="rId433" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
+    <hyperlink ref="B356" r:id="rId434" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
+    <hyperlink ref="B2" r:id="rId435" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
+    <hyperlink ref="B95" r:id="rId436" xr:uid="{1F507CBC-4056-AD46-9314-95ECBB9D799D}"/>
+    <hyperlink ref="B94" r:id="rId437" xr:uid="{AB28D9E6-890C-F14A-A5FB-2303BE319968}"/>
+    <hyperlink ref="B93" r:id="rId438" xr:uid="{B9AC5194-6D36-684A-A5C4-BEE11037599F}"/>
+    <hyperlink ref="B92" r:id="rId439" xr:uid="{C8C607BB-1FEE-FA47-9E3E-6C0BCE978B7F}"/>
+    <hyperlink ref="B91" r:id="rId440" xr:uid="{2D956AC4-4774-7446-8473-C4CE00E33C17}"/>
+    <hyperlink ref="B90" r:id="rId441" xr:uid="{ED0F5FC7-0066-EB44-8FCF-460600DADB02}"/>
+    <hyperlink ref="B89" r:id="rId442" xr:uid="{A3D51762-65A1-9A44-B619-D1D98A7F403B}"/>
+    <hyperlink ref="B88" r:id="rId443" xr:uid="{8E3D4BDF-9F8F-0542-BFD8-C3CE3BF396E6}"/>
+    <hyperlink ref="B87" r:id="rId444" xr:uid="{62982242-1D19-1544-8653-8E25E9BF4505}"/>
+    <hyperlink ref="B292" r:id="rId445" xr:uid="{E3384259-7CA7-1C44-A66D-11346EE6742E}"/>
+    <hyperlink ref="B374" r:id="rId446" xr:uid="{A35F55D4-9B87-C745-94DB-E7D820193C30}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId447"/>

</xml_diff>

<commit_message>
Day 88 and 89
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783B09A5-9924-4DAE-8CE5-BEEB8F60B43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA397F2-859F-4943-AED8-1816C559F0A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1971,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A369" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C380" sqref="C380"/>
+    <sheetView tabSelected="1" topLeftCell="A382" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C388" sqref="C388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5984,8 +5984,8 @@
       <c r="B382" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="C382" s="4" t="s">
-        <v>4</v>
+      <c r="C382" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="383" spans="1:3" ht="21">
@@ -5995,8 +5995,8 @@
       <c r="B383" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="C383" s="4" t="s">
-        <v>4</v>
+      <c r="C383" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="384" spans="1:3" ht="21">
@@ -6006,8 +6006,8 @@
       <c r="B384" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="C384" s="4" t="s">
-        <v>4</v>
+      <c r="C384" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="385" spans="1:3" ht="21">
@@ -6017,8 +6017,8 @@
       <c r="B385" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="C385" s="4" t="s">
-        <v>4</v>
+      <c r="C385" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="386" spans="1:3" ht="21">
@@ -6028,8 +6028,8 @@
       <c r="B386" s="6" t="s">
         <v>374</v>
       </c>
-      <c r="C386" s="4" t="s">
-        <v>4</v>
+      <c r="C386" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="387" spans="1:3" ht="21">
@@ -6039,8 +6039,8 @@
       <c r="B387" s="6" t="s">
         <v>375</v>
       </c>
-      <c r="C387" s="4" t="s">
-        <v>4</v>
+      <c r="C387" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="388" spans="1:3" ht="21">
@@ -6050,8 +6050,8 @@
       <c r="B388" s="6" t="s">
         <v>376</v>
       </c>
-      <c r="C388" s="4" t="s">
-        <v>4</v>
+      <c r="C388" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="389" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 92 to 97
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E562CA-0909-4148-9F7A-4D7116CB2489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5CA439-6ED3-4799-B3F3-FC01E94363D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1971,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A388" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C399" sqref="C399"/>
+    <sheetView tabSelected="1" topLeftCell="A406" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C415" sqref="C415"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6264,8 +6264,8 @@
       <c r="B410" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="C410" s="4" t="s">
-        <v>4</v>
+      <c r="C410" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="411" spans="1:3" ht="21">
@@ -6275,8 +6275,8 @@
       <c r="B411" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="C411" s="4" t="s">
-        <v>4</v>
+      <c r="C411" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="412" spans="1:3" ht="21">
@@ -6286,8 +6286,8 @@
       <c r="B412" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="C412" s="4" t="s">
-        <v>4</v>
+      <c r="C412" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="413" spans="1:3" ht="21">
@@ -6297,8 +6297,8 @@
       <c r="B413" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="C413" s="4" t="s">
-        <v>4</v>
+      <c r="C413" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="414" spans="1:3" ht="21">
@@ -6308,8 +6308,8 @@
       <c r="B414" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="C414" s="4" t="s">
-        <v>4</v>
+      <c r="C414" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="415" spans="1:3" ht="21">
@@ -6319,8 +6319,8 @@
       <c r="B415" s="6" t="s">
         <v>399</v>
       </c>
-      <c r="C415" s="4" t="s">
-        <v>4</v>
+      <c r="C415" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="416" spans="1:3" ht="21">
@@ -6330,8 +6330,8 @@
       <c r="B416" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="C416" s="4" t="s">
-        <v>4</v>
+      <c r="C416" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="417" spans="1:3" ht="21">
@@ -6341,8 +6341,8 @@
       <c r="B417" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="C417" s="4" t="s">
-        <v>4</v>
+      <c r="C417" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="418" spans="1:3" ht="21">
@@ -6352,8 +6352,8 @@
       <c r="B418" s="6" t="s">
         <v>401</v>
       </c>
-      <c r="C418" s="4" t="s">
-        <v>4</v>
+      <c r="C418" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="419" spans="1:3" ht="21">
@@ -6363,8 +6363,8 @@
       <c r="B419" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="C419" s="4" t="s">
-        <v>4</v>
+      <c r="C419" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="420" spans="1:3" ht="21">
@@ -6374,8 +6374,8 @@
       <c r="B420" s="6" t="s">
         <v>403</v>
       </c>
-      <c r="C420" s="4" t="s">
-        <v>4</v>
+      <c r="C420" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="421" spans="1:3" ht="21">
@@ -6385,8 +6385,8 @@
       <c r="B421" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="C421" s="4" t="s">
-        <v>4</v>
+      <c r="C421" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="422" spans="1:3" ht="21">
@@ -6396,8 +6396,8 @@
       <c r="B422" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="C422" s="4" t="s">
-        <v>4</v>
+      <c r="C422" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="423" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 98 and 99
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5CA439-6ED3-4799-B3F3-FC01E94363D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC428BA-D35A-4203-A49E-6E576F62C485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1971,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A406" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C415" sqref="C415"/>
+    <sheetView tabSelected="1" topLeftCell="A418" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C429" sqref="C429"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6407,8 +6407,8 @@
       <c r="B423" s="6" t="s">
         <v>406</v>
       </c>
-      <c r="C423" s="4" t="s">
-        <v>4</v>
+      <c r="C423" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="424" spans="1:3" ht="21">
@@ -6418,8 +6418,8 @@
       <c r="B424" s="6" t="s">
         <v>407</v>
       </c>
-      <c r="C424" s="4" t="s">
-        <v>4</v>
+      <c r="C424" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="425" spans="1:3" ht="21">
@@ -6429,8 +6429,8 @@
       <c r="B425" s="6" t="s">
         <v>408</v>
       </c>
-      <c r="C425" s="4" t="s">
-        <v>4</v>
+      <c r="C425" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="426" spans="1:3" ht="21">
@@ -6440,8 +6440,8 @@
       <c r="B426" s="6" t="s">
         <v>409</v>
       </c>
-      <c r="C426" s="4" t="s">
-        <v>4</v>
+      <c r="C426" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="427" spans="1:3" ht="21">
@@ -6451,8 +6451,8 @@
       <c r="B427" s="6" t="s">
         <v>410</v>
       </c>
-      <c r="C427" s="4" t="s">
-        <v>4</v>
+      <c r="C427" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="428" spans="1:3" ht="21">
@@ -6462,8 +6462,8 @@
       <c r="B428" s="6" t="s">
         <v>411</v>
       </c>
-      <c r="C428" s="4" t="s">
-        <v>4</v>
+      <c r="C428" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="429" spans="1:3" ht="21">
@@ -6473,8 +6473,8 @@
       <c r="B429" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="C429" s="4" t="s">
-        <v>4</v>
+      <c r="C429" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="430" spans="1:3" ht="21">
@@ -6484,8 +6484,8 @@
       <c r="B430" s="6" t="s">
         <v>413</v>
       </c>
-      <c r="C430" s="4" t="s">
-        <v>4</v>
+      <c r="C430" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="431" spans="1:3" ht="21">
@@ -6495,8 +6495,8 @@
       <c r="B431" s="6" t="s">
         <v>414</v>
       </c>
-      <c r="C431" s="4" t="s">
-        <v>4</v>
+      <c r="C431" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="432" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 100, 101 and 102
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC428BA-D35A-4203-A49E-6E576F62C485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97BE74D-1C45-4DB1-B41D-E261D63E5756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1971,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A418" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C429" sqref="C429"/>
+    <sheetView tabSelected="1" topLeftCell="A457" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B450" sqref="B450"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6506,8 +6506,8 @@
       <c r="B432" s="6" t="s">
         <v>415</v>
       </c>
-      <c r="C432" s="4" t="s">
-        <v>4</v>
+      <c r="C432" s="13" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="433" spans="1:3" ht="21">
@@ -6517,8 +6517,8 @@
       <c r="B433" s="6" t="s">
         <v>416</v>
       </c>
-      <c r="C433" s="4" t="s">
-        <v>4</v>
+      <c r="C433" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="434" spans="1:3" ht="21">
@@ -6528,8 +6528,8 @@
       <c r="B434" s="6" t="s">
         <v>417</v>
       </c>
-      <c r="C434" s="4" t="s">
-        <v>4</v>
+      <c r="C434" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="435" spans="1:3" ht="21">
@@ -6539,8 +6539,8 @@
       <c r="B435" s="6" t="s">
         <v>418</v>
       </c>
-      <c r="C435" s="4" t="s">
-        <v>4</v>
+      <c r="C435" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="436" spans="1:3" ht="21">
@@ -6550,8 +6550,8 @@
       <c r="B436" s="6" t="s">
         <v>419</v>
       </c>
-      <c r="C436" s="4" t="s">
-        <v>4</v>
+      <c r="C436" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="437" spans="1:3" ht="21">
@@ -6561,8 +6561,8 @@
       <c r="B437" s="6" t="s">
         <v>420</v>
       </c>
-      <c r="C437" s="4" t="s">
-        <v>4</v>
+      <c r="C437" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="438" spans="1:3" ht="21">
@@ -6572,8 +6572,8 @@
       <c r="B438" s="6" t="s">
         <v>421</v>
       </c>
-      <c r="C438" s="4" t="s">
-        <v>4</v>
+      <c r="C438" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="439" spans="1:3" ht="21">
@@ -6583,8 +6583,8 @@
       <c r="B439" s="6" t="s">
         <v>422</v>
       </c>
-      <c r="C439" s="4" t="s">
-        <v>4</v>
+      <c r="C439" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="440" spans="1:3" ht="21">
@@ -6594,8 +6594,8 @@
       <c r="B440" s="6" t="s">
         <v>423</v>
       </c>
-      <c r="C440" s="4" t="s">
-        <v>4</v>
+      <c r="C440" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="441" spans="1:3" ht="21">
@@ -6605,8 +6605,8 @@
       <c r="B441" s="6" t="s">
         <v>424</v>
       </c>
-      <c r="C441" s="4" t="s">
-        <v>4</v>
+      <c r="C441" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="442" spans="1:3" ht="21">
@@ -6616,8 +6616,8 @@
       <c r="B442" s="6" t="s">
         <v>425</v>
       </c>
-      <c r="C442" s="4" t="s">
-        <v>4</v>
+      <c r="C442" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="443" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 104 and 105
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9513B5-9E48-49A4-BC5D-CD62A8061040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9112145-6746-4EAE-857B-79FEACF08904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1971,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A442" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C450" sqref="C450"/>
+    <sheetView tabSelected="1" topLeftCell="A445" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C455" sqref="C455"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6704,8 +6704,8 @@
       <c r="B450" s="6" t="s">
         <v>433</v>
       </c>
-      <c r="C450" s="4" t="s">
-        <v>4</v>
+      <c r="C450" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="451" spans="1:3" ht="21">
@@ -6715,8 +6715,8 @@
       <c r="B451" s="6" t="s">
         <v>434</v>
       </c>
-      <c r="C451" s="4" t="s">
-        <v>4</v>
+      <c r="C451" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="452" spans="1:3" ht="21">
@@ -6726,8 +6726,8 @@
       <c r="B452" s="6" t="s">
         <v>435</v>
       </c>
-      <c r="C452" s="4" t="s">
-        <v>4</v>
+      <c r="C452" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="453" spans="1:3" ht="21">
@@ -6737,8 +6737,8 @@
       <c r="B453" s="6" t="s">
         <v>436</v>
       </c>
-      <c r="C453" s="4" t="s">
-        <v>4</v>
+      <c r="C453" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="454" spans="1:3" ht="21">
@@ -6748,8 +6748,8 @@
       <c r="B454" s="6" t="s">
         <v>437</v>
       </c>
-      <c r="C454" s="4" t="s">
-        <v>4</v>
+      <c r="C454" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="455" spans="1:3" ht="21">
@@ -6759,8 +6759,8 @@
       <c r="B455" s="6" t="s">
         <v>438</v>
       </c>
-      <c r="C455" s="4" t="s">
-        <v>4</v>
+      <c r="C455" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="456" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 106 and 107
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9112145-6746-4EAE-857B-79FEACF08904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD698CB-C1C2-4BE7-B906-F62DD094D504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1971,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A445" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C455" sqref="C455"/>
+    <sheetView tabSelected="1" topLeftCell="A451" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C462" sqref="C462"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6770,8 +6770,8 @@
       <c r="B456" s="6" t="s">
         <v>439</v>
       </c>
-      <c r="C456" s="4" t="s">
-        <v>4</v>
+      <c r="C456" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="457" spans="1:3" ht="21">
@@ -6781,8 +6781,8 @@
       <c r="B457" s="6" t="s">
         <v>440</v>
       </c>
-      <c r="C457" s="4" t="s">
-        <v>4</v>
+      <c r="C457" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="458" spans="1:3" ht="21">
@@ -6792,8 +6792,8 @@
       <c r="B458" s="6" t="s">
         <v>441</v>
       </c>
-      <c r="C458" s="4" t="s">
-        <v>4</v>
+      <c r="C458" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="459" spans="1:3" ht="21">
@@ -6803,8 +6803,8 @@
       <c r="B459" s="6" t="s">
         <v>442</v>
       </c>
-      <c r="C459" s="4" t="s">
-        <v>4</v>
+      <c r="C459" s="20" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="460" spans="1:3" ht="21">
@@ -6814,8 +6814,8 @@
       <c r="B460" s="6" t="s">
         <v>443</v>
       </c>
-      <c r="C460" s="4" t="s">
-        <v>4</v>
+      <c r="C460" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="461" spans="1:3" ht="21">
@@ -6825,8 +6825,8 @@
       <c r="B461" s="6" t="s">
         <v>444</v>
       </c>
-      <c r="C461" s="4" t="s">
-        <v>4</v>
+      <c r="C461" s="13" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="462" spans="1:3" ht="21">
@@ -6836,8 +6836,8 @@
       <c r="B462" s="6" t="s">
         <v>445</v>
       </c>
-      <c r="C462" s="4" t="s">
-        <v>4</v>
+      <c r="C462" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="463" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 109 and 110
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EF9DF9-AC93-4783-B2BF-9D2343966BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E99651-BF05-4A98-AEA6-7AC1DB4B8CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1971,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A456" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B465" sqref="B465"/>
+    <sheetView tabSelected="1" topLeftCell="A174" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C178" sqref="C178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3811,8 +3811,8 @@
       <c r="B177" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="C177" s="4" t="s">
-        <v>4</v>
+      <c r="C177" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="21">
@@ -3822,8 +3822,8 @@
       <c r="B178" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="C178" s="4" t="s">
-        <v>4</v>
+      <c r="C178" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="21">
@@ -3833,8 +3833,8 @@
       <c r="B179" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C179" s="4" t="s">
-        <v>4</v>
+      <c r="C179" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="21">
@@ -3844,8 +3844,8 @@
       <c r="B180" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C180" s="4" t="s">
-        <v>4</v>
+      <c r="C180" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="21">
@@ -3855,8 +3855,8 @@
       <c r="B181" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="C181" s="4" t="s">
-        <v>4</v>
+      <c r="C181" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="21">
@@ -3866,8 +3866,8 @@
       <c r="B182" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C182" s="4" t="s">
-        <v>4</v>
+      <c r="C182" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="21">
@@ -3877,8 +3877,8 @@
       <c r="B183" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="C183" s="4" t="s">
-        <v>4</v>
+      <c r="C183" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="21">
@@ -3888,8 +3888,8 @@
       <c r="B184" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C184" s="4" t="s">
-        <v>4</v>
+      <c r="C184" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="21">
@@ -3899,8 +3899,8 @@
       <c r="B185" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="C185" s="4" t="s">
-        <v>4</v>
+      <c r="C185" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="21">
@@ -3910,8 +3910,8 @@
       <c r="B186" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="C186" s="4" t="s">
-        <v>4</v>
+      <c r="C186" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="21">
@@ -3921,8 +3921,8 @@
       <c r="B187" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="C187" s="4" t="s">
-        <v>4</v>
+      <c r="C187" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="21">
@@ -3932,8 +3932,8 @@
       <c r="B188" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="C188" s="4" t="s">
-        <v>4</v>
+      <c r="C188" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="21">
@@ -3943,8 +3943,8 @@
       <c r="B189" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="C189" s="4" t="s">
-        <v>4</v>
+      <c r="C189" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="21">
@@ -3954,8 +3954,8 @@
       <c r="B190" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="C190" s="4" t="s">
-        <v>4</v>
+      <c r="C190" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="21">
@@ -3965,8 +3965,8 @@
       <c r="B191" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="C191" s="4" t="s">
-        <v>4</v>
+      <c r="C191" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="21">
@@ -3976,8 +3976,8 @@
       <c r="B192" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C192" s="4" t="s">
-        <v>4</v>
+      <c r="C192" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 111 to 115 Binary Tree Completed
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E99651-BF05-4A98-AEA6-7AC1DB4B8CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034C69E4-0A49-48F8-8496-D7006FFEE493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="471">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1441,6 +1441,9 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>NEED BST</t>
   </si>
 </sst>
 </file>
@@ -1971,8 +1974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C178" sqref="C178"/>
+    <sheetView tabSelected="1" topLeftCell="A196" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C209" sqref="A177:C211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3987,8 +3990,8 @@
       <c r="B193" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="C193" s="4" t="s">
-        <v>4</v>
+      <c r="C193" s="13" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="21">
@@ -3998,8 +4001,8 @@
       <c r="B194" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C194" s="4" t="s">
-        <v>4</v>
+      <c r="C194" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="21">
@@ -4009,8 +4012,8 @@
       <c r="B195" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="C195" s="4" t="s">
-        <v>4</v>
+      <c r="C195" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="21">
@@ -4020,8 +4023,8 @@
       <c r="B196" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="C196" s="4" t="s">
-        <v>4</v>
+      <c r="C196" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="197" spans="1:3" ht="21">
@@ -4031,8 +4034,8 @@
       <c r="B197" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="C197" s="4" t="s">
-        <v>4</v>
+      <c r="C197" s="20" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="21">
@@ -4042,8 +4045,8 @@
       <c r="B198" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="C198" s="4" t="s">
-        <v>4</v>
+      <c r="C198" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="21">
@@ -4053,8 +4056,8 @@
       <c r="B199" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C199" s="4" t="s">
-        <v>4</v>
+      <c r="C199" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="21">
@@ -4064,8 +4067,8 @@
       <c r="B200" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C200" s="4" t="s">
-        <v>4</v>
+      <c r="C200" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="21">
@@ -4075,8 +4078,8 @@
       <c r="B201" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="C201" s="4" t="s">
-        <v>4</v>
+      <c r="C201" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="21">
@@ -4086,8 +4089,8 @@
       <c r="B202" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C202" s="4" t="s">
-        <v>4</v>
+      <c r="C202" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="21">
@@ -4097,8 +4100,8 @@
       <c r="B203" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="C203" s="4" t="s">
-        <v>4</v>
+      <c r="C203" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="21">
@@ -4108,8 +4111,8 @@
       <c r="B204" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="C204" s="4" t="s">
-        <v>4</v>
+      <c r="C204" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="205" spans="1:3" ht="21">
@@ -4119,8 +4122,8 @@
       <c r="B205" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="C205" s="4" t="s">
-        <v>4</v>
+      <c r="C205" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="21">
@@ -4130,8 +4133,8 @@
       <c r="B206" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="C206" s="4" t="s">
-        <v>4</v>
+      <c r="C206" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="207" spans="1:3" ht="21">
@@ -4141,8 +4144,8 @@
       <c r="B207" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="C207" s="4" t="s">
-        <v>4</v>
+      <c r="C207" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="208" spans="1:3" ht="21">
@@ -4152,8 +4155,8 @@
       <c r="B208" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="C208" s="4" t="s">
-        <v>4</v>
+      <c r="C208" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="209" spans="1:3" ht="21">
@@ -4163,8 +4166,8 @@
       <c r="B209" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="C209" s="4" t="s">
-        <v>4</v>
+      <c r="C209" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="210" spans="1:3" ht="21">
@@ -4174,8 +4177,8 @@
       <c r="B210" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="C210" s="4" t="s">
-        <v>4</v>
+      <c r="C210" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="211" spans="1:3" ht="21">
@@ -4185,8 +4188,8 @@
       <c r="B211" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="C211" s="4" t="s">
-        <v>4</v>
+      <c r="C211" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="212" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 116 to Day 120 Binary Search Tree Completed
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034C69E4-0A49-48F8-8496-D7006FFEE493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F248198-92D1-48FF-8764-D204947AA4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1974,8 +1974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C209" sqref="A177:C211"/>
+    <sheetView tabSelected="1" topLeftCell="A220" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C234" sqref="C234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -4209,8 +4209,8 @@
       <c r="B214" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="C214" s="4" t="s">
-        <v>4</v>
+      <c r="C214" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="21">
@@ -4220,8 +4220,8 @@
       <c r="B215" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="C215" s="4" t="s">
-        <v>4</v>
+      <c r="C215" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="216" spans="1:3" ht="21">
@@ -4231,8 +4231,8 @@
       <c r="B216" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="C216" s="4" t="s">
-        <v>4</v>
+      <c r="C216" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="21">
@@ -4242,8 +4242,8 @@
       <c r="B217" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C217" s="4" t="s">
-        <v>4</v>
+      <c r="C217" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="21">
@@ -4253,8 +4253,8 @@
       <c r="B218" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C218" s="4" t="s">
-        <v>4</v>
+      <c r="C218" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="219" spans="1:3" ht="21">
@@ -4264,8 +4264,8 @@
       <c r="B219" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="C219" s="4" t="s">
-        <v>4</v>
+      <c r="C219" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="220" spans="1:3" ht="21">
@@ -4275,8 +4275,8 @@
       <c r="B220" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="C220" s="4" t="s">
-        <v>4</v>
+      <c r="C220" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="221" spans="1:3" ht="21">
@@ -4286,8 +4286,8 @@
       <c r="B221" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="C221" s="4" t="s">
-        <v>4</v>
+      <c r="C221" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="222" spans="1:3" ht="21">
@@ -4297,8 +4297,8 @@
       <c r="B222" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="C222" s="4" t="s">
-        <v>4</v>
+      <c r="C222" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="21">
@@ -4308,8 +4308,8 @@
       <c r="B223" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="C223" s="4" t="s">
-        <v>4</v>
+      <c r="C223" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="21">
@@ -4319,8 +4319,8 @@
       <c r="B224" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="C224" s="4" t="s">
-        <v>4</v>
+      <c r="C224" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="225" spans="1:3" ht="21">
@@ -4330,8 +4330,8 @@
       <c r="B225" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="C225" s="4" t="s">
-        <v>4</v>
+      <c r="C225" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="226" spans="1:3" ht="21">
@@ -4341,8 +4341,8 @@
       <c r="B226" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="C226" s="4" t="s">
-        <v>4</v>
+      <c r="C226" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="227" spans="1:3" ht="21">
@@ -4352,8 +4352,8 @@
       <c r="B227" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="C227" s="4" t="s">
-        <v>4</v>
+      <c r="C227" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="228" spans="1:3" ht="21">
@@ -4363,8 +4363,8 @@
       <c r="B228" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="C228" s="4" t="s">
-        <v>4</v>
+      <c r="C228" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="21">
@@ -4374,8 +4374,8 @@
       <c r="B229" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="C229" s="4" t="s">
-        <v>4</v>
+      <c r="C229" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="21">
@@ -4385,8 +4385,8 @@
       <c r="B230" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C230" s="4" t="s">
-        <v>4</v>
+      <c r="C230" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="21">
@@ -4396,8 +4396,8 @@
       <c r="B231" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="C231" s="4" t="s">
-        <v>4</v>
+      <c r="C231" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="232" spans="1:3" ht="21">
@@ -4407,8 +4407,8 @@
       <c r="B232" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="C232" s="4" t="s">
-        <v>4</v>
+      <c r="C232" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="21">
@@ -4418,8 +4418,8 @@
       <c r="B233" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="C233" s="4" t="s">
-        <v>4</v>
+      <c r="C233" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="234" spans="1:3" ht="21">
@@ -4429,8 +4429,8 @@
       <c r="B234" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="C234" s="4" t="s">
-        <v>4</v>
+      <c r="C234" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="235" spans="1:3" ht="21">
@@ -4440,8 +4440,8 @@
       <c r="B235" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="C235" s="4" t="s">
-        <v>4</v>
+      <c r="C235" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="236" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 122 to Day 123
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CAC2E3-B655-45FA-B16F-71CF637DB660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C56BCC-0FE6-44D5-8E8E-B52B8E20CCFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1974,8 +1974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A298" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B307" sqref="B307:B308"/>
+    <sheetView tabSelected="1" topLeftCell="A301" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B307" sqref="B307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5168,8 +5168,8 @@
       <c r="B305" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="C305" s="4" t="s">
-        <v>4</v>
+      <c r="C305" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="306" spans="1:3" ht="21">
@@ -5179,8 +5179,8 @@
       <c r="B306" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="C306" s="4" t="s">
-        <v>4</v>
+      <c r="C306" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="307" spans="1:3" ht="21">
@@ -5190,8 +5190,8 @@
       <c r="B307" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="C307" s="4" t="s">
-        <v>4</v>
+      <c r="C307" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="308" spans="1:3" ht="21">
@@ -5201,8 +5201,8 @@
       <c r="B308" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="C308" s="4" t="s">
-        <v>4</v>
+      <c r="C308" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="309" spans="1:3" ht="21">
@@ -5212,8 +5212,8 @@
       <c r="B309" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="C309" s="4" t="s">
-        <v>4</v>
+      <c r="C309" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="310" spans="1:3" ht="21">
@@ -5223,8 +5223,8 @@
       <c r="B310" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="C310" s="4" t="s">
-        <v>4</v>
+      <c r="C310" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="311" spans="1:3" ht="21">
@@ -5234,8 +5234,8 @@
       <c r="B311" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="C311" s="4" t="s">
-        <v>4</v>
+      <c r="C311" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="312" spans="1:3" ht="21">
@@ -5245,8 +5245,8 @@
       <c r="B312" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="C312" s="4" t="s">
-        <v>4</v>
+      <c r="C312" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="313" spans="1:3" ht="21">
@@ -5256,8 +5256,8 @@
       <c r="B313" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="C313" s="4" t="s">
-        <v>4</v>
+      <c r="C313" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="314" spans="1:3" ht="21">
@@ -5267,8 +5267,8 @@
       <c r="B314" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="C314" s="4" t="s">
-        <v>4</v>
+      <c r="C314" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="315" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 126 to 130 Heap Completed
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0543D8-15C3-4FFD-BB07-21158D5A89FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5125B602-EB64-4429-A1CA-83DD716FFC45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1974,8 +1974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A322" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C328" sqref="C328"/>
+    <sheetView tabSelected="1" topLeftCell="A329" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C350" sqref="C350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5495,8 +5495,8 @@
       <c r="B336" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="C336" s="4" t="s">
-        <v>4</v>
+      <c r="C336" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="337" spans="1:3" ht="21">
@@ -5506,8 +5506,8 @@
       <c r="B337" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="C337" s="4" t="s">
-        <v>4</v>
+      <c r="C337" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="338" spans="1:3" ht="21">
@@ -5517,8 +5517,8 @@
       <c r="B338" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="C338" s="4" t="s">
-        <v>4</v>
+      <c r="C338" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="339" spans="1:3" ht="21">
@@ -5528,8 +5528,8 @@
       <c r="B339" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="C339" s="4" t="s">
-        <v>4</v>
+      <c r="C339" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="340" spans="1:3" ht="21">
@@ -5539,8 +5539,8 @@
       <c r="B340" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="C340" s="4" t="s">
-        <v>4</v>
+      <c r="C340" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="341" spans="1:3" ht="21">
@@ -5550,8 +5550,8 @@
       <c r="B341" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="C341" s="4" t="s">
-        <v>4</v>
+      <c r="C341" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="342" spans="1:3" ht="21">
@@ -5561,8 +5561,8 @@
       <c r="B342" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="C342" s="4" t="s">
-        <v>4</v>
+      <c r="C342" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="343" spans="1:3" ht="21">
@@ -5572,8 +5572,8 @@
       <c r="B343" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="C343" s="4" t="s">
-        <v>4</v>
+      <c r="C343" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="344" spans="1:3" ht="21">
@@ -5583,8 +5583,8 @@
       <c r="B344" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="C344" s="4" t="s">
-        <v>4</v>
+      <c r="C344" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="345" spans="1:3" ht="21">
@@ -5594,8 +5594,8 @@
       <c r="B345" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="C345" s="4" t="s">
-        <v>4</v>
+      <c r="C345" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="346" spans="1:3" ht="21">
@@ -5605,8 +5605,8 @@
       <c r="B346" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="C346" s="4" t="s">
-        <v>4</v>
+      <c r="C346" s="13" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="347" spans="1:3" ht="21">
@@ -5616,8 +5616,8 @@
       <c r="B347" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="C347" s="4" t="s">
-        <v>4</v>
+      <c r="C347" s="13" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="348" spans="1:3" ht="21">
@@ -5627,8 +5627,8 @@
       <c r="B348" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="C348" s="4" t="s">
-        <v>4</v>
+      <c r="C348" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="349" spans="1:3" ht="21">
@@ -5638,8 +5638,8 @@
       <c r="B349" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="C349" s="4" t="s">
-        <v>4</v>
+      <c r="C349" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="350" spans="1:3" ht="21">
@@ -5649,8 +5649,8 @@
       <c r="B350" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="C350" s="4" t="s">
-        <v>4</v>
+      <c r="C350" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="351" spans="1:3" ht="21">
@@ -5660,8 +5660,8 @@
       <c r="B351" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="C351" s="4" t="s">
-        <v>4</v>
+      <c r="C351" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="352" spans="1:3" ht="21">
@@ -5671,8 +5671,8 @@
       <c r="B352" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="C352" s="4" t="s">
-        <v>4</v>
+      <c r="C352" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="353" spans="1:3" ht="21">
@@ -5682,8 +5682,8 @@
       <c r="B353" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="C353" s="4" t="s">
-        <v>4</v>
+      <c r="C353" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="354" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 131 to 133 Trie Completed
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5125B602-EB64-4429-A1CA-83DD716FFC45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7852A8-FF7F-432A-92E5-86BCE55281FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1974,8 +1974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A329" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C350" sqref="C350"/>
+    <sheetView tabSelected="1" topLeftCell="A398" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B402" sqref="B402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6193,8 +6193,8 @@
       <c r="B402" s="6" t="s">
         <v>388</v>
       </c>
-      <c r="C402" s="4" t="s">
-        <v>4</v>
+      <c r="C402" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="403" spans="1:3" ht="21">
@@ -6204,8 +6204,8 @@
       <c r="B403" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="C403" s="4" t="s">
-        <v>4</v>
+      <c r="C403" s="13" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="404" spans="1:3" ht="21">
@@ -6215,8 +6215,8 @@
       <c r="B404" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="C404" s="4" t="s">
-        <v>4</v>
+      <c r="C404" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="405" spans="1:3" ht="21">
@@ -6226,8 +6226,8 @@
       <c r="B405" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C405" s="4" t="s">
-        <v>4</v>
+      <c r="C405" s="13" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="406" spans="1:3" ht="21">
@@ -6237,8 +6237,8 @@
       <c r="B406" s="6" t="s">
         <v>391</v>
       </c>
-      <c r="C406" s="4" t="s">
-        <v>4</v>
+      <c r="C406" s="13" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="407" spans="1:3" ht="21">
@@ -6248,8 +6248,8 @@
       <c r="B407" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="C407" s="4" t="s">
-        <v>4</v>
+      <c r="C407" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="408" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day 134 to 136 Bit Manipulation Completed
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Sheets\lovebabbar-dsa-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7852A8-FF7F-432A-92E5-86BCE55281FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166ED467-7F9A-4B82-8F29-38A0869D9D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1974,8 +1974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A398" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B402" sqref="B402"/>
+    <sheetView tabSelected="1" topLeftCell="A470" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C474" sqref="C474"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6936,8 +6936,8 @@
       <c r="B472" s="6" t="s">
         <v>454</v>
       </c>
-      <c r="C472" s="4" t="s">
-        <v>4</v>
+      <c r="C472" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="473" spans="1:3" ht="21">
@@ -6947,8 +6947,8 @@
       <c r="B473" s="6" t="s">
         <v>455</v>
       </c>
-      <c r="C473" s="4" t="s">
-        <v>4</v>
+      <c r="C473" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="474" spans="1:3" ht="21">
@@ -6958,8 +6958,8 @@
       <c r="B474" s="6" t="s">
         <v>456</v>
       </c>
-      <c r="C474" s="4" t="s">
-        <v>4</v>
+      <c r="C474" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="475" spans="1:3" ht="21">
@@ -6969,8 +6969,8 @@
       <c r="B475" s="6" t="s">
         <v>457</v>
       </c>
-      <c r="C475" s="4" t="s">
-        <v>4</v>
+      <c r="C475" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="476" spans="1:3" ht="21">
@@ -6980,8 +6980,8 @@
       <c r="B476" s="6" t="s">
         <v>458</v>
       </c>
-      <c r="C476" s="4" t="s">
-        <v>4</v>
+      <c r="C476" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="477" spans="1:3" ht="21">
@@ -6991,8 +6991,8 @@
       <c r="B477" s="6" t="s">
         <v>459</v>
       </c>
-      <c r="C477" s="4" t="s">
-        <v>4</v>
+      <c r="C477" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="478" spans="1:3" ht="21">
@@ -7002,8 +7002,8 @@
       <c r="B478" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="C478" s="4" t="s">
-        <v>4</v>
+      <c r="C478" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="479" spans="1:3" ht="21">
@@ -7013,8 +7013,8 @@
       <c r="B479" s="6" t="s">
         <v>461</v>
       </c>
-      <c r="C479" s="4" t="s">
-        <v>4</v>
+      <c r="C479" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="480" spans="1:3" ht="21">
@@ -7024,8 +7024,8 @@
       <c r="B480" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="C480" s="4" t="s">
-        <v>4</v>
+      <c r="C480" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="481" spans="1:3" ht="21">
@@ -7035,8 +7035,8 @@
       <c r="B481" s="6" t="s">
         <v>463</v>
       </c>
-      <c r="C481" s="4" t="s">
-        <v>4</v>
+      <c r="C481" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>